<commit_message>
Updated with data from 3/22/2020
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C06A986D-FC1F-0B45-AD46-AF813A6A8A3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA727F0-68E8-764E-A3CC-249C5A710183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29040" yWindow="-2560" windowWidth="17380" windowHeight="12920" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-31880" yWindow="-2480" windowWidth="31360" windowHeight="16760" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BQ$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BS$17</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>date</t>
   </si>
@@ -244,6 +243,12 @@
   </si>
   <si>
     <t>ranchosantafe</t>
+  </si>
+  <si>
+    <t>lamesa</t>
+  </si>
+  <si>
+    <t>lakeside</t>
   </si>
 </sst>
 </file>
@@ -596,20 +601,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BQ17"/>
+  <dimension ref="A1:BS18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="BL8" sqref="BL8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="52" max="52" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,40 +790,46 @@
         <v>57</v>
       </c>
       <c r="BG1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BH1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BR1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BS1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43896</v>
       </c>
@@ -832,32 +843,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43897</v>
       </c>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
     </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
     </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43900</v>
       </c>
     </row>
-    <row r="7" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43901</v>
       </c>
     </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
@@ -871,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43903</v>
       </c>
@@ -885,12 +896,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43904</v>
       </c>
     </row>
-    <row r="11" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43905</v>
       </c>
@@ -958,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43906</v>
       </c>
@@ -1026,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43907</v>
       </c>
@@ -1094,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43908</v>
       </c>
@@ -1162,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43909</v>
       </c>
@@ -1311,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43910</v>
       </c>
@@ -1460,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43911</v>
       </c>
@@ -1635,26 +1646,23 @@
       <c r="BF17">
         <v>2</v>
       </c>
-      <c r="BG17">
-        <v>1</v>
-      </c>
       <c r="BH17">
+        <v>1</v>
+      </c>
+      <c r="BI17">
         <v>4</v>
       </c>
-      <c r="BI17">
-        <v>1</v>
-      </c>
       <c r="BJ17">
+        <v>1</v>
+      </c>
+      <c r="BK17">
         <v>87</v>
       </c>
-      <c r="BK17">
-        <v>3</v>
-      </c>
       <c r="BL17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BM17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BN17">
         <v>2</v>
@@ -1665,76 +1673,226 @@
       <c r="BP17">
         <v>2</v>
       </c>
-      <c r="BQ17">
+      <c r="BR17">
+        <v>2</v>
+      </c>
+      <c r="BS17">
         <v>2</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC65B7E-9E39-1F44-8678-1537799ECFFD}">
-  <dimension ref="A1:Q1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="A1:Q1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="18" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B18">
+        <v>178</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="F18">
         <v>49</v>
       </c>
-      <c r="P1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>51</v>
+      <c r="G18">
+        <v>33</v>
+      </c>
+      <c r="H18">
+        <v>27</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>15</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>61</v>
+      </c>
+      <c r="N18">
+        <v>116</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>32</v>
+      </c>
+      <c r="Q18">
+        <v>14</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>11</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>4</v>
+      </c>
+      <c r="AA18">
+        <v>2</v>
+      </c>
+      <c r="AB18">
+        <v>5</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>4</v>
+      </c>
+      <c r="AE18">
+        <v>7</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>6</v>
+      </c>
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <v>0</v>
+      </c>
+      <c r="AJ18">
+        <v>16</v>
+      </c>
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18">
+        <v>1</v>
+      </c>
+      <c r="AM18">
+        <v>6</v>
+      </c>
+      <c r="AN18">
+        <v>3</v>
+      </c>
+      <c r="AO18">
+        <v>2</v>
+      </c>
+      <c r="AP18">
+        <v>0</v>
+      </c>
+      <c r="AQ18">
+        <v>1</v>
+      </c>
+      <c r="AR18">
+        <v>3</v>
+      </c>
+      <c r="AS18">
+        <v>0</v>
+      </c>
+      <c r="AT18">
+        <v>0</v>
+      </c>
+      <c r="AU18">
+        <v>6</v>
+      </c>
+      <c r="AV18">
+        <v>10</v>
+      </c>
+      <c r="AW18">
+        <v>0</v>
+      </c>
+      <c r="AX18">
+        <v>3</v>
+      </c>
+      <c r="AY18">
+        <v>1</v>
+      </c>
+      <c r="AZ18">
+        <v>0</v>
+      </c>
+      <c r="BA18">
+        <v>12</v>
+      </c>
+      <c r="BB18">
+        <v>4</v>
+      </c>
+      <c r="BC18">
+        <v>4</v>
+      </c>
+      <c r="BD18">
+        <v>2</v>
+      </c>
+      <c r="BE18">
+        <v>5</v>
+      </c>
+      <c r="BF18">
+        <v>3</v>
+      </c>
+      <c r="BG18">
+        <v>1</v>
+      </c>
+      <c r="BH18">
+        <v>2</v>
+      </c>
+      <c r="BI18">
+        <v>4</v>
+      </c>
+      <c r="BJ18">
+        <v>2</v>
+      </c>
+      <c r="BK18">
+        <v>118</v>
+      </c>
+      <c r="BL18">
+        <v>3</v>
+      </c>
+      <c r="BM18">
+        <v>1</v>
+      </c>
+      <c r="BN18">
+        <v>2</v>
+      </c>
+      <c r="BO18">
+        <v>2</v>
+      </c>
+      <c r="BP18">
+        <v>2</v>
+      </c>
+      <c r="BQ18">
+        <v>1</v>
+      </c>
+      <c r="BR18">
+        <v>2</v>
+      </c>
+      <c r="BS18">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated w/ data from 23Mar2020
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA727F0-68E8-764E-A3CC-249C5A710183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7050923E-9C1B-3144-A819-D1ED167B51CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31880" yWindow="-2480" windowWidth="31360" windowHeight="16760" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-19000" yWindow="-3600" windowWidth="19000" windowHeight="21600" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BS$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BT$17</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>date</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>lakeside</t>
+  </si>
+  <si>
+    <t>bonita</t>
+  </si>
+  <si>
+    <t>springvalley</t>
   </si>
 </sst>
 </file>
@@ -601,20 +607,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BS18"/>
+  <dimension ref="A1:BU19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
-      <selection activeCell="BL8" sqref="BL8"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
+      <selection activeCell="BU19" sqref="BU19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="52" max="52" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,19 +823,25 @@
         <v>65</v>
       </c>
       <c r="BP1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BQ1" t="s">
         <v>66</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>70</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>67</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>68</v>
       </c>
+      <c r="BU1" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43896</v>
       </c>
@@ -843,32 +855,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43897</v>
       </c>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43900</v>
       </c>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43901</v>
       </c>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
@@ -882,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43903</v>
       </c>
@@ -896,12 +908,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43904</v>
       </c>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43905</v>
       </c>
@@ -969,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43906</v>
       </c>
@@ -1037,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43907</v>
       </c>
@@ -1105,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43908</v>
       </c>
@@ -1173,7 +1185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43909</v>
       </c>
@@ -1322,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43910</v>
       </c>
@@ -1471,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43911</v>
       </c>
@@ -1670,17 +1682,17 @@
       <c r="BO17">
         <v>2</v>
       </c>
-      <c r="BP17">
-        <v>2</v>
-      </c>
-      <c r="BR17">
+      <c r="BQ17">
         <v>2</v>
       </c>
       <c r="BS17">
         <v>2</v>
       </c>
+      <c r="BT17">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43912</v>
       </c>
@@ -1882,17 +1894,187 @@
       <c r="BO18">
         <v>2</v>
       </c>
-      <c r="BP18">
-        <v>2</v>
-      </c>
       <c r="BQ18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BR18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BS18">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="BT18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:73" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B19">
+        <v>213</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>46</v>
+      </c>
+      <c r="F19">
+        <v>59</v>
+      </c>
+      <c r="G19">
+        <v>39</v>
+      </c>
+      <c r="H19">
+        <v>32</v>
+      </c>
+      <c r="I19">
+        <v>13</v>
+      </c>
+      <c r="J19">
+        <v>15</v>
+      </c>
+      <c r="K19">
+        <v>6</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>78</v>
+      </c>
+      <c r="N19">
+        <v>134</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>34</v>
+      </c>
+      <c r="Q19">
+        <v>17</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="AJ19">
+        <v>17</v>
+      </c>
+      <c r="AK19">
+        <v>0</v>
+      </c>
+      <c r="AL19">
+        <v>1</v>
+      </c>
+      <c r="AM19">
+        <v>7</v>
+      </c>
+      <c r="AN19">
+        <v>3</v>
+      </c>
+      <c r="AO19">
+        <v>2</v>
+      </c>
+      <c r="AP19">
+        <v>0</v>
+      </c>
+      <c r="AQ19">
+        <v>1</v>
+      </c>
+      <c r="AR19">
+        <v>3</v>
+      </c>
+      <c r="AS19">
+        <v>0</v>
+      </c>
+      <c r="AT19">
+        <v>0</v>
+      </c>
+      <c r="AU19">
+        <v>6</v>
+      </c>
+      <c r="AV19">
+        <v>11</v>
+      </c>
+      <c r="AW19">
+        <v>0</v>
+      </c>
+      <c r="AX19">
+        <v>3</v>
+      </c>
+      <c r="AY19">
+        <v>1</v>
+      </c>
+      <c r="AZ19">
+        <v>0</v>
+      </c>
+      <c r="BA19">
+        <v>14</v>
+      </c>
+      <c r="BB19">
+        <v>6</v>
+      </c>
+      <c r="BC19">
+        <v>5</v>
+      </c>
+      <c r="BD19">
+        <v>7</v>
+      </c>
+      <c r="BE19">
+        <v>5</v>
+      </c>
+      <c r="BF19">
+        <v>5</v>
+      </c>
+      <c r="BG19">
+        <v>1</v>
+      </c>
+      <c r="BH19">
+        <v>3</v>
+      </c>
+      <c r="BI19">
+        <v>5</v>
+      </c>
+      <c r="BJ19">
+        <v>2</v>
+      </c>
+      <c r="BK19">
+        <v>134</v>
+      </c>
+      <c r="BL19">
+        <v>3</v>
+      </c>
+      <c r="BM19">
+        <v>1</v>
+      </c>
+      <c r="BN19">
+        <v>1</v>
+      </c>
+      <c r="BO19">
+        <v>2</v>
+      </c>
+      <c r="BP19">
+        <v>1</v>
+      </c>
+      <c r="BQ19">
+        <v>2</v>
+      </c>
+      <c r="BR19">
+        <v>2</v>
+      </c>
+      <c r="BS19">
+        <v>2</v>
+      </c>
+      <c r="BT19">
+        <v>5</v>
+      </c>
+      <c r="BU19">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data up to Mar 25
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7050923E-9C1B-3144-A819-D1ED167B51CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FBE2E8-A794-B44A-A7BA-2828CF374B7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19000" yWindow="-3600" windowWidth="19000" windowHeight="21600" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-37040" yWindow="-3140" windowWidth="28800" windowHeight="17540" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BT$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BV$17</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>date</t>
   </si>
@@ -255,6 +255,15 @@
   </si>
   <si>
     <t>springvalley</t>
+  </si>
+  <si>
+    <t>lemongrove</t>
+  </si>
+  <si>
+    <t>jamul</t>
+  </si>
+  <si>
+    <t>sanysidro</t>
   </si>
 </sst>
 </file>
@@ -607,20 +616,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BU19"/>
+  <dimension ref="A1:BX21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="BU19" sqref="BU19"/>
+    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
+      <selection activeCell="BW21" sqref="BW21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="52" max="52" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,49 +809,58 @@
         <v>69</v>
       </c>
       <c r="BH1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI1" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>65</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>71</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>66</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BT1" t="s">
         <v>70</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BU1" t="s">
         <v>67</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BV1" t="s">
         <v>68</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BW1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BX1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43896</v>
       </c>
@@ -855,32 +874,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43897</v>
       </c>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43900</v>
       </c>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43901</v>
       </c>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
@@ -894,7 +913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43903</v>
       </c>
@@ -908,12 +927,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43904</v>
       </c>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43905</v>
       </c>
@@ -981,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43906</v>
       </c>
@@ -1049,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43907</v>
       </c>
@@ -1117,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43908</v>
       </c>
@@ -1185,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43909</v>
       </c>
@@ -1334,7 +1353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43910</v>
       </c>
@@ -1483,7 +1502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43911</v>
       </c>
@@ -1658,41 +1677,41 @@
       <c r="BF17">
         <v>2</v>
       </c>
-      <c r="BH17">
-        <v>1</v>
-      </c>
       <c r="BI17">
+        <v>1</v>
+      </c>
+      <c r="BJ17">
         <v>4</v>
       </c>
-      <c r="BJ17">
-        <v>1</v>
-      </c>
       <c r="BK17">
+        <v>1</v>
+      </c>
+      <c r="BL17">
         <v>87</v>
       </c>
-      <c r="BL17">
-        <v>3</v>
-      </c>
       <c r="BM17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BN17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BO17">
         <v>2</v>
       </c>
-      <c r="BQ17">
-        <v>2</v>
-      </c>
-      <c r="BS17">
-        <v>2</v>
-      </c>
-      <c r="BT17">
+      <c r="BP17">
+        <v>2</v>
+      </c>
+      <c r="BR17">
+        <v>2</v>
+      </c>
+      <c r="BU17">
+        <v>2</v>
+      </c>
+      <c r="BV17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43912</v>
       </c>
@@ -1870,44 +1889,44 @@
       <c r="BG18">
         <v>1</v>
       </c>
-      <c r="BH18">
-        <v>2</v>
-      </c>
       <c r="BI18">
+        <v>2</v>
+      </c>
+      <c r="BJ18">
         <v>4</v>
       </c>
-      <c r="BJ18">
-        <v>2</v>
-      </c>
       <c r="BK18">
+        <v>2</v>
+      </c>
+      <c r="BL18">
         <v>118</v>
       </c>
-      <c r="BL18">
-        <v>3</v>
-      </c>
       <c r="BM18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BN18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BO18">
         <v>2</v>
       </c>
-      <c r="BQ18">
+      <c r="BP18">
         <v>2</v>
       </c>
       <c r="BR18">
-        <v>1</v>
-      </c>
-      <c r="BS18">
         <v>2</v>
       </c>
       <c r="BT18">
+        <v>1</v>
+      </c>
+      <c r="BU18">
+        <v>2</v>
+      </c>
+      <c r="BV18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43913</v>
       </c>
@@ -2034,47 +2053,396 @@
       <c r="BG19">
         <v>1</v>
       </c>
-      <c r="BH19">
-        <v>3</v>
-      </c>
       <c r="BI19">
+        <v>3</v>
+      </c>
+      <c r="BJ19">
         <v>5</v>
       </c>
-      <c r="BJ19">
-        <v>2</v>
-      </c>
       <c r="BK19">
+        <v>2</v>
+      </c>
+      <c r="BL19">
         <v>134</v>
       </c>
-      <c r="BL19">
-        <v>3</v>
-      </c>
       <c r="BM19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BN19">
         <v>1</v>
       </c>
       <c r="BO19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BP19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BQ19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BR19">
         <v>2</v>
       </c>
-      <c r="BS19">
-        <v>2</v>
-      </c>
       <c r="BT19">
+        <v>2</v>
+      </c>
+      <c r="BU19">
+        <v>2</v>
+      </c>
+      <c r="BV19">
         <v>5</v>
       </c>
-      <c r="BU19">
-        <v>2</v>
+      <c r="BX19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B20">
+        <v>226</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>46</v>
+      </c>
+      <c r="F20">
+        <v>63</v>
+      </c>
+      <c r="G20">
+        <v>41</v>
+      </c>
+      <c r="H20">
+        <v>33</v>
+      </c>
+      <c r="I20">
+        <v>17</v>
+      </c>
+      <c r="J20">
+        <v>15</v>
+      </c>
+      <c r="K20">
+        <v>7</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>80</v>
+      </c>
+      <c r="N20">
+        <v>146</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>44</v>
+      </c>
+      <c r="Q20">
+        <v>20</v>
+      </c>
+      <c r="R20">
+        <v>2</v>
+      </c>
+      <c r="AJ20">
+        <v>16</v>
+      </c>
+      <c r="AK20">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <v>1</v>
+      </c>
+      <c r="AM20">
+        <v>8</v>
+      </c>
+      <c r="AN20">
+        <v>3</v>
+      </c>
+      <c r="AO20">
+        <v>2</v>
+      </c>
+      <c r="AP20">
+        <v>0</v>
+      </c>
+      <c r="AQ20">
+        <v>1</v>
+      </c>
+      <c r="AR20">
+        <v>1</v>
+      </c>
+      <c r="AS20">
+        <v>0</v>
+      </c>
+      <c r="AT20">
+        <v>0</v>
+      </c>
+      <c r="AU20">
+        <v>5</v>
+      </c>
+      <c r="AV20">
+        <v>11</v>
+      </c>
+      <c r="AW20">
+        <v>0</v>
+      </c>
+      <c r="AX20">
+        <v>1</v>
+      </c>
+      <c r="AY20">
+        <v>1</v>
+      </c>
+      <c r="AZ20">
+        <v>0</v>
+      </c>
+      <c r="BA20">
+        <v>13</v>
+      </c>
+      <c r="BB20">
+        <v>7</v>
+      </c>
+      <c r="BC20">
+        <v>5</v>
+      </c>
+      <c r="BD20">
+        <v>8</v>
+      </c>
+      <c r="BE20">
+        <v>7</v>
+      </c>
+      <c r="BF20">
+        <v>6</v>
+      </c>
+      <c r="BG20">
+        <v>1</v>
+      </c>
+      <c r="BI20">
+        <v>3</v>
+      </c>
+      <c r="BJ20">
+        <v>7</v>
+      </c>
+      <c r="BK20">
+        <v>2</v>
+      </c>
+      <c r="BL20">
+        <v>141</v>
+      </c>
+      <c r="BM20">
+        <v>3</v>
+      </c>
+      <c r="BN20">
+        <v>1</v>
+      </c>
+      <c r="BO20">
+        <v>1</v>
+      </c>
+      <c r="BP20">
+        <v>2</v>
+      </c>
+      <c r="BQ20">
+        <v>1</v>
+      </c>
+      <c r="BR20">
+        <v>2</v>
+      </c>
+      <c r="BT20">
+        <v>2</v>
+      </c>
+      <c r="BU20">
+        <v>2</v>
+      </c>
+      <c r="BV20">
+        <v>5</v>
+      </c>
+      <c r="BX20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B21">
+        <v>277</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>55</v>
+      </c>
+      <c r="F21">
+        <v>74</v>
+      </c>
+      <c r="G21">
+        <v>51</v>
+      </c>
+      <c r="H21">
+        <v>40</v>
+      </c>
+      <c r="I21">
+        <v>23</v>
+      </c>
+      <c r="J21">
+        <v>19</v>
+      </c>
+      <c r="K21">
+        <v>11</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>107</v>
+      </c>
+      <c r="N21">
+        <v>170</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>57</v>
+      </c>
+      <c r="Q21">
+        <v>28</v>
+      </c>
+      <c r="R21">
+        <v>2</v>
+      </c>
+      <c r="AJ21">
+        <v>20</v>
+      </c>
+      <c r="AK21">
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <v>1</v>
+      </c>
+      <c r="AM21">
+        <v>10</v>
+      </c>
+      <c r="AN21">
+        <v>3</v>
+      </c>
+      <c r="AO21">
+        <v>3</v>
+      </c>
+      <c r="AP21">
+        <v>0</v>
+      </c>
+      <c r="AQ21">
+        <v>1</v>
+      </c>
+      <c r="AR21">
+        <v>1</v>
+      </c>
+      <c r="AS21">
+        <v>1</v>
+      </c>
+      <c r="AT21">
+        <v>0</v>
+      </c>
+      <c r="AU21">
+        <v>5</v>
+      </c>
+      <c r="AV21">
+        <v>15</v>
+      </c>
+      <c r="AW21">
+        <v>0</v>
+      </c>
+      <c r="AX21">
+        <v>2</v>
+      </c>
+      <c r="AY21">
+        <v>1</v>
+      </c>
+      <c r="AZ21">
+        <v>0</v>
+      </c>
+      <c r="BA21">
+        <v>16</v>
+      </c>
+      <c r="BB21">
+        <v>13</v>
+      </c>
+      <c r="BC21">
+        <v>5</v>
+      </c>
+      <c r="BD21">
+        <v>13</v>
+      </c>
+      <c r="BE21">
+        <v>8</v>
+      </c>
+      <c r="BF21">
+        <v>6</v>
+      </c>
+      <c r="BG21">
+        <v>1</v>
+      </c>
+      <c r="BH21">
+        <v>1</v>
+      </c>
+      <c r="BI21">
+        <v>5</v>
+      </c>
+      <c r="BJ21">
+        <v>7</v>
+      </c>
+      <c r="BK21">
+        <v>3</v>
+      </c>
+      <c r="BL21">
+        <v>169</v>
+      </c>
+      <c r="BM21">
+        <v>3</v>
+      </c>
+      <c r="BN21">
+        <v>1</v>
+      </c>
+      <c r="BO21">
+        <v>1</v>
+      </c>
+      <c r="BP21">
+        <v>3</v>
+      </c>
+      <c r="BQ21">
+        <v>1</v>
+      </c>
+      <c r="BR21">
+        <v>2</v>
+      </c>
+      <c r="BS21">
+        <v>1</v>
+      </c>
+      <c r="BT21">
+        <v>2</v>
+      </c>
+      <c r="BU21">
+        <v>2</v>
+      </c>
+      <c r="BV21">
+        <v>5</v>
+      </c>
+      <c r="BW21">
+        <v>1</v>
+      </c>
+      <c r="BX21">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with 27 March data
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0560FED7-032E-F64C-8A90-FD4C35789C49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEED2C5B-EAB3-B64E-9EEC-BA7AA3DDEA75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36060" yWindow="-3140" windowWidth="32920" windowHeight="18960" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="1980" yWindow="460" windowWidth="24220" windowHeight="17540" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AX$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AY$17</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>date</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>sd_70to79_hosp</t>
+  </si>
+  <si>
+    <t>coronado</t>
   </si>
 </sst>
 </file>
@@ -538,21 +541,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:AZ22"/>
+  <dimension ref="A1:BA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="BB23" sqref="BB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12.83203125" customWidth="1"/>
+    <col min="51" max="51" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,83 +647,86 @@
         <v>19</v>
       </c>
       <c r="AE1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" t="s">
         <v>20</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>21</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>22</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>23</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>39</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>24</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>27</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>28</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>29</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>30</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>31</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>37</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>32</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>36</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>33</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>34</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>41</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43896</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43897</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
@@ -728,7 +734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
@@ -736,7 +742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43900</v>
       </c>
@@ -744,7 +750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43901</v>
       </c>
@@ -752,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
@@ -760,7 +766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43903</v>
       </c>
@@ -768,7 +774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43904</v>
       </c>
@@ -776,7 +782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43905</v>
       </c>
@@ -784,7 +790,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43906</v>
       </c>
@@ -792,7 +798,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43907</v>
       </c>
@@ -800,7 +806,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43908</v>
       </c>
@@ -808,7 +814,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43909</v>
       </c>
@@ -816,7 +822,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43910</v>
       </c>
@@ -824,7 +830,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43911</v>
       </c>
@@ -837,53 +843,53 @@
       <c r="AD17">
         <v>4</v>
       </c>
-      <c r="AE17">
-        <v>2</v>
-      </c>
       <c r="AF17">
         <v>2</v>
       </c>
       <c r="AG17">
+        <v>2</v>
+      </c>
+      <c r="AH17">
         <v>4</v>
       </c>
-      <c r="AH17">
-        <v>2</v>
-      </c>
-      <c r="AK17">
-        <v>1</v>
+      <c r="AI17">
+        <v>2</v>
       </c>
       <c r="AL17">
+        <v>1</v>
+      </c>
+      <c r="AM17">
         <v>4</v>
       </c>
-      <c r="AM17">
-        <v>1</v>
-      </c>
       <c r="AN17">
+        <v>1</v>
+      </c>
+      <c r="AO17">
         <v>87</v>
       </c>
-      <c r="AO17">
-        <v>3</v>
-      </c>
       <c r="AP17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AQ17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR17">
         <v>2</v>
       </c>
-      <c r="AT17">
-        <v>2</v>
-      </c>
-      <c r="AW17">
+      <c r="AS17">
+        <v>2</v>
+      </c>
+      <c r="AU17">
         <v>2</v>
       </c>
       <c r="AX17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="AY17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43912</v>
       </c>
@@ -896,59 +902,59 @@
       <c r="AD18">
         <v>4</v>
       </c>
-      <c r="AE18">
+      <c r="AF18">
         <v>4</v>
       </c>
-      <c r="AF18">
-        <v>2</v>
-      </c>
       <c r="AG18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AH18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AI18">
-        <v>1</v>
-      </c>
-      <c r="AK18">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="AJ18">
+        <v>1</v>
       </c>
       <c r="AL18">
+        <v>2</v>
+      </c>
+      <c r="AM18">
         <v>4</v>
       </c>
-      <c r="AM18">
-        <v>2</v>
-      </c>
       <c r="AN18">
+        <v>2</v>
+      </c>
+      <c r="AO18">
         <v>118</v>
       </c>
-      <c r="AO18">
-        <v>3</v>
-      </c>
       <c r="AP18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AQ18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR18">
         <v>2</v>
       </c>
-      <c r="AT18">
-        <v>2</v>
-      </c>
-      <c r="AV18">
-        <v>1</v>
+      <c r="AS18">
+        <v>2</v>
+      </c>
+      <c r="AU18">
+        <v>2</v>
       </c>
       <c r="AW18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AX18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="AY18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43913</v>
       </c>
@@ -961,65 +967,65 @@
       <c r="AD19">
         <v>6</v>
       </c>
-      <c r="AE19">
-        <v>5</v>
-      </c>
       <c r="AF19">
+        <v>5</v>
+      </c>
+      <c r="AG19">
         <v>7</v>
       </c>
-      <c r="AG19">
-        <v>5</v>
-      </c>
       <c r="AH19">
         <v>5</v>
       </c>
       <c r="AI19">
-        <v>1</v>
-      </c>
-      <c r="AK19">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="AJ19">
+        <v>1</v>
       </c>
       <c r="AL19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AN19">
+        <v>2</v>
+      </c>
+      <c r="AO19">
         <v>134</v>
       </c>
-      <c r="AO19">
-        <v>3</v>
-      </c>
       <c r="AP19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AQ19">
         <v>1</v>
       </c>
       <c r="AR19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT19">
-        <v>2</v>
-      </c>
-      <c r="AV19">
+        <v>1</v>
+      </c>
+      <c r="AU19">
         <v>2</v>
       </c>
       <c r="AW19">
         <v>2</v>
       </c>
       <c r="AX19">
-        <v>5</v>
-      </c>
-      <c r="AZ19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="AY19">
+        <v>5</v>
+      </c>
+      <c r="BA19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43914</v>
       </c>
@@ -1032,65 +1038,65 @@
       <c r="AD20">
         <v>7</v>
       </c>
-      <c r="AE20">
-        <v>5</v>
-      </c>
       <c r="AF20">
+        <v>5</v>
+      </c>
+      <c r="AG20">
         <v>8</v>
       </c>
-      <c r="AG20">
+      <c r="AH20">
         <v>7</v>
       </c>
-      <c r="AH20">
+      <c r="AI20">
         <v>6</v>
       </c>
-      <c r="AI20">
-        <v>1</v>
-      </c>
-      <c r="AK20">
-        <v>3</v>
+      <c r="AJ20">
+        <v>1</v>
       </c>
       <c r="AL20">
+        <v>3</v>
+      </c>
+      <c r="AM20">
         <v>7</v>
       </c>
-      <c r="AM20">
-        <v>2</v>
-      </c>
       <c r="AN20">
+        <v>2</v>
+      </c>
+      <c r="AO20">
         <v>141</v>
       </c>
-      <c r="AO20">
-        <v>3</v>
-      </c>
       <c r="AP20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AQ20">
         <v>1</v>
       </c>
       <c r="AR20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT20">
-        <v>2</v>
-      </c>
-      <c r="AV20">
+        <v>1</v>
+      </c>
+      <c r="AU20">
         <v>2</v>
       </c>
       <c r="AW20">
         <v>2</v>
       </c>
       <c r="AX20">
-        <v>5</v>
-      </c>
-      <c r="AZ20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="AY20">
+        <v>5</v>
+      </c>
+      <c r="BA20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43915</v>
       </c>
@@ -1103,74 +1109,74 @@
       <c r="AD21">
         <v>13</v>
       </c>
-      <c r="AE21">
-        <v>5</v>
-      </c>
       <c r="AF21">
+        <v>5</v>
+      </c>
+      <c r="AG21">
         <v>13</v>
       </c>
-      <c r="AG21">
+      <c r="AH21">
         <v>8</v>
       </c>
-      <c r="AH21">
+      <c r="AI21">
         <v>6</v>
       </c>
-      <c r="AI21">
-        <v>1</v>
-      </c>
       <c r="AJ21">
         <v>1</v>
       </c>
       <c r="AK21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AL21">
+        <v>5</v>
+      </c>
+      <c r="AM21">
         <v>7</v>
       </c>
-      <c r="AM21">
-        <v>3</v>
-      </c>
       <c r="AN21">
+        <v>3</v>
+      </c>
+      <c r="AO21">
         <v>169</v>
       </c>
-      <c r="AO21">
-        <v>3</v>
-      </c>
       <c r="AP21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AQ21">
         <v>1</v>
       </c>
       <c r="AR21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AS21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AT21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AU21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AV21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW21">
         <v>2</v>
       </c>
       <c r="AX21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AY21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AZ21">
+        <v>1</v>
+      </c>
+      <c r="BA21">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43916</v>
       </c>
@@ -1258,65 +1264,190 @@
       <c r="AD22">
         <v>17</v>
       </c>
-      <c r="AE22">
-        <v>5</v>
-      </c>
       <c r="AF22">
+        <v>5</v>
+      </c>
+      <c r="AG22">
         <v>19</v>
       </c>
-      <c r="AG22">
+      <c r="AH22">
         <v>12</v>
       </c>
-      <c r="AH22">
+      <c r="AI22">
         <v>7</v>
       </c>
-      <c r="AI22">
-        <v>1</v>
-      </c>
       <c r="AJ22">
         <v>1</v>
       </c>
       <c r="AK22">
+        <v>1</v>
+      </c>
+      <c r="AL22">
         <v>6</v>
       </c>
-      <c r="AL22">
+      <c r="AM22">
         <v>8</v>
       </c>
-      <c r="AM22">
+      <c r="AN22">
         <v>4</v>
       </c>
-      <c r="AN22">
+      <c r="AO22">
         <v>207</v>
       </c>
-      <c r="AO22">
-        <v>3</v>
-      </c>
       <c r="AP22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AQ22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AS22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AT22">
-        <v>2</v>
-      </c>
-      <c r="AV22">
+        <v>1</v>
+      </c>
+      <c r="AU22">
         <v>2</v>
       </c>
       <c r="AW22">
         <v>2</v>
       </c>
       <c r="AX22">
-        <v>5</v>
-      </c>
-      <c r="AZ22">
+        <v>2</v>
+      </c>
+      <c r="AY22">
+        <v>5</v>
+      </c>
+      <c r="BA22">
         <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B23">
+        <v>417</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>84</v>
+      </c>
+      <c r="I23">
+        <v>106</v>
+      </c>
+      <c r="K23">
+        <v>73</v>
+      </c>
+      <c r="M23">
+        <v>65</v>
+      </c>
+      <c r="O23">
+        <v>31</v>
+      </c>
+      <c r="Q23">
+        <v>29</v>
+      </c>
+      <c r="S23">
+        <v>20</v>
+      </c>
+      <c r="U23">
+        <v>2</v>
+      </c>
+      <c r="W23">
+        <v>166</v>
+      </c>
+      <c r="X23">
+        <v>249</v>
+      </c>
+      <c r="Y23">
+        <v>2</v>
+      </c>
+      <c r="Z23">
+        <v>85</v>
+      </c>
+      <c r="AA23">
+        <v>38</v>
+      </c>
+      <c r="AB23">
+        <v>5</v>
+      </c>
+      <c r="AC23">
+        <v>18</v>
+      </c>
+      <c r="AD23">
+        <v>21</v>
+      </c>
+      <c r="AE23">
+        <v>1</v>
+      </c>
+      <c r="AF23">
+        <v>6</v>
+      </c>
+      <c r="AG23">
+        <v>20</v>
+      </c>
+      <c r="AH23">
+        <v>14</v>
+      </c>
+      <c r="AI23">
+        <v>7</v>
+      </c>
+      <c r="AJ23">
+        <v>3</v>
+      </c>
+      <c r="AK23">
+        <v>1</v>
+      </c>
+      <c r="AL23">
+        <v>6</v>
+      </c>
+      <c r="AM23">
+        <v>8</v>
+      </c>
+      <c r="AN23">
+        <v>5</v>
+      </c>
+      <c r="AO23">
+        <v>251</v>
+      </c>
+      <c r="AP23">
+        <v>3</v>
+      </c>
+      <c r="AQ23">
+        <v>2</v>
+      </c>
+      <c r="AR23">
+        <v>1</v>
+      </c>
+      <c r="AS23">
+        <v>6</v>
+      </c>
+      <c r="AT23">
+        <v>2</v>
+      </c>
+      <c r="AU23">
+        <v>3</v>
+      </c>
+      <c r="AW23">
+        <v>2</v>
+      </c>
+      <c r="AX23">
+        <v>3</v>
+      </c>
+      <c r="AY23">
+        <v>6</v>
+      </c>
+      <c r="BA23">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with data from Mar 28, 2020
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEED2C5B-EAB3-B64E-9EEC-BA7AA3DDEA75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA1E5F2-1ADA-714A-B488-4C051DB9D896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="460" windowWidth="24220" windowHeight="17540" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-34220" yWindow="-1760" windowWidth="24220" windowHeight="17540" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BA23"/>
+  <dimension ref="A1:BA24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="BB23" sqref="BB23"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1450,6 +1450,161 @@
         <v>5</v>
       </c>
     </row>
+    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>43918</v>
+      </c>
+      <c r="B24">
+        <v>488</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>102</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <v>118</v>
+      </c>
+      <c r="J24">
+        <v>14</v>
+      </c>
+      <c r="K24">
+        <v>85</v>
+      </c>
+      <c r="L24">
+        <v>15</v>
+      </c>
+      <c r="M24">
+        <v>74</v>
+      </c>
+      <c r="N24">
+        <v>21</v>
+      </c>
+      <c r="O24">
+        <v>36</v>
+      </c>
+      <c r="P24">
+        <v>12</v>
+      </c>
+      <c r="Q24">
+        <v>38</v>
+      </c>
+      <c r="R24">
+        <v>13</v>
+      </c>
+      <c r="S24">
+        <v>25</v>
+      </c>
+      <c r="T24">
+        <v>15</v>
+      </c>
+      <c r="U24">
+        <v>2</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>206</v>
+      </c>
+      <c r="X24">
+        <v>280</v>
+      </c>
+      <c r="Y24">
+        <v>2</v>
+      </c>
+      <c r="Z24">
+        <v>96</v>
+      </c>
+      <c r="AA24">
+        <v>42</v>
+      </c>
+      <c r="AB24">
+        <v>7</v>
+      </c>
+      <c r="AC24">
+        <v>19</v>
+      </c>
+      <c r="AD24">
+        <v>24</v>
+      </c>
+      <c r="AE24">
+        <v>1</v>
+      </c>
+      <c r="AF24">
+        <v>6</v>
+      </c>
+      <c r="AG24">
+        <v>26</v>
+      </c>
+      <c r="AH24">
+        <v>16</v>
+      </c>
+      <c r="AI24">
+        <v>9</v>
+      </c>
+      <c r="AJ24">
+        <v>3</v>
+      </c>
+      <c r="AK24">
+        <v>2</v>
+      </c>
+      <c r="AL24">
+        <v>8</v>
+      </c>
+      <c r="AM24">
+        <v>11</v>
+      </c>
+      <c r="AN24">
+        <v>7</v>
+      </c>
+      <c r="AO24">
+        <v>284</v>
+      </c>
+      <c r="AP24">
+        <v>3</v>
+      </c>
+      <c r="AQ24">
+        <v>2</v>
+      </c>
+      <c r="AR24">
+        <v>1</v>
+      </c>
+      <c r="AS24">
+        <v>10</v>
+      </c>
+      <c r="AT24">
+        <v>2</v>
+      </c>
+      <c r="AU24">
+        <v>4</v>
+      </c>
+      <c r="AW24">
+        <v>2</v>
+      </c>
+      <c r="AX24">
+        <v>4</v>
+      </c>
+      <c r="AY24">
+        <v>7</v>
+      </c>
+      <c r="BA24">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated w/ Mar 29 data
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA1E5F2-1ADA-714A-B488-4C051DB9D896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA98C8F6-0927-B448-9541-66DB4B518C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34220" yWindow="-1760" windowWidth="24220" windowHeight="17540" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AY$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AZ$17</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>date</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>coronado</t>
+  </si>
+  <si>
+    <t>tested</t>
   </si>
 </sst>
 </file>
@@ -224,9 +227,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,1067 +545,1241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BA24"/>
+  <dimension ref="A1:BB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BD25" sqref="BD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
       <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
       <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>46</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>49</v>
-      </c>
-      <c r="S1" t="s">
-        <v>10</v>
       </c>
       <c r="T1" t="s">
         <v>10</v>
       </c>
       <c r="U1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="V1" t="s">
         <v>13</v>
       </c>
       <c r="W1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" t="s">
         <v>11</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>17</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>18</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>19</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>50</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>20</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>21</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>22</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>39</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>25</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>26</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>27</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>28</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>29</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>30</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>31</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>37</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>32</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>40</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>36</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>33</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>34</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>41</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43896</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43897</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43900</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43901</v>
       </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43903</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
+        <v>52</v>
+      </c>
+      <c r="C9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43904</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
+        <v>14</v>
+      </c>
+      <c r="C10">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43905</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43906</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
+        <v>25</v>
+      </c>
+      <c r="C12">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43907</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
+        <v>77</v>
+      </c>
+      <c r="C13">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43908</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
+        <v>143</v>
+      </c>
+      <c r="C14">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43909</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
+        <v>320</v>
+      </c>
+      <c r="C15">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43910</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
+        <v>93</v>
+      </c>
+      <c r="C16">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43911</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
+        <v>788</v>
+      </c>
+      <c r="C17">
         <v>118</v>
       </c>
-      <c r="AC17">
+      <c r="AD17">
         <v>11</v>
       </c>
-      <c r="AD17">
-        <v>4</v>
-      </c>
-      <c r="AF17">
-        <v>2</v>
+      <c r="AE17">
+        <v>4</v>
       </c>
       <c r="AG17">
         <v>2</v>
       </c>
       <c r="AH17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI17">
-        <v>2</v>
-      </c>
-      <c r="AL17">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="AJ17">
+        <v>2</v>
       </c>
       <c r="AM17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AN17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AO17">
+        <v>1</v>
+      </c>
+      <c r="AP17">
         <v>87</v>
       </c>
-      <c r="AP17">
-        <v>3</v>
-      </c>
       <c r="AQ17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AR17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS17">
         <v>2</v>
       </c>
-      <c r="AU17">
-        <v>2</v>
-      </c>
-      <c r="AX17">
+      <c r="AT17">
+        <v>2</v>
+      </c>
+      <c r="AV17">
         <v>2</v>
       </c>
       <c r="AY17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="AZ17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43912</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
+        <v>422</v>
+      </c>
+      <c r="C18">
         <v>143</v>
       </c>
-      <c r="AC18">
+      <c r="AD18">
         <v>12</v>
       </c>
-      <c r="AD18">
-        <v>4</v>
-      </c>
-      <c r="AF18">
+      <c r="AE18">
         <v>4</v>
       </c>
       <c r="AG18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AI18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AJ18">
-        <v>1</v>
-      </c>
-      <c r="AL18">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="AK18">
+        <v>1</v>
       </c>
       <c r="AM18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AN18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AO18">
+        <v>2</v>
+      </c>
+      <c r="AP18">
         <v>118</v>
       </c>
-      <c r="AP18">
-        <v>3</v>
-      </c>
       <c r="AQ18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AR18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS18">
         <v>2</v>
       </c>
-      <c r="AU18">
-        <v>2</v>
-      </c>
-      <c r="AW18">
-        <v>1</v>
+      <c r="AT18">
+        <v>2</v>
+      </c>
+      <c r="AV18">
+        <v>2</v>
       </c>
       <c r="AX18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AY18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="AZ18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43913</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
+        <v>382</v>
+      </c>
+      <c r="C19">
         <v>197</v>
       </c>
-      <c r="AC19">
+      <c r="AD19">
         <v>14</v>
       </c>
-      <c r="AD19">
+      <c r="AE19">
         <v>6</v>
       </c>
-      <c r="AF19">
-        <v>5</v>
-      </c>
       <c r="AG19">
+        <v>5</v>
+      </c>
+      <c r="AH19">
         <v>7</v>
       </c>
-      <c r="AH19">
-        <v>5</v>
-      </c>
       <c r="AI19">
         <v>5</v>
       </c>
       <c r="AJ19">
-        <v>1</v>
-      </c>
-      <c r="AL19">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="AK19">
+        <v>1</v>
       </c>
       <c r="AM19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AN19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AO19">
+        <v>2</v>
+      </c>
+      <c r="AP19">
         <v>134</v>
       </c>
-      <c r="AP19">
-        <v>3</v>
-      </c>
       <c r="AQ19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AR19">
         <v>1</v>
       </c>
       <c r="AS19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AU19">
-        <v>2</v>
-      </c>
-      <c r="AW19">
+        <v>1</v>
+      </c>
+      <c r="AV19">
         <v>2</v>
       </c>
       <c r="AX19">
         <v>2</v>
       </c>
       <c r="AY19">
-        <v>5</v>
-      </c>
-      <c r="BA19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="AZ19">
+        <v>5</v>
+      </c>
+      <c r="BB19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43914</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
+        <v>504</v>
+      </c>
+      <c r="C20">
         <v>232</v>
       </c>
-      <c r="AC20">
+      <c r="AD20">
         <v>13</v>
       </c>
-      <c r="AD20">
+      <c r="AE20">
         <v>7</v>
       </c>
-      <c r="AF20">
-        <v>5</v>
-      </c>
       <c r="AG20">
+        <v>5</v>
+      </c>
+      <c r="AH20">
         <v>8</v>
       </c>
-      <c r="AH20">
+      <c r="AI20">
         <v>7</v>
       </c>
-      <c r="AI20">
+      <c r="AJ20">
         <v>6</v>
       </c>
-      <c r="AJ20">
-        <v>1</v>
-      </c>
-      <c r="AL20">
-        <v>3</v>
+      <c r="AK20">
+        <v>1</v>
       </c>
       <c r="AM20">
+        <v>3</v>
+      </c>
+      <c r="AN20">
         <v>7</v>
       </c>
-      <c r="AN20">
-        <v>2</v>
-      </c>
       <c r="AO20">
+        <v>2</v>
+      </c>
+      <c r="AP20">
         <v>141</v>
       </c>
-      <c r="AP20">
-        <v>3</v>
-      </c>
       <c r="AQ20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AR20">
         <v>1</v>
       </c>
       <c r="AS20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AU20">
-        <v>2</v>
-      </c>
-      <c r="AW20">
+        <v>1</v>
+      </c>
+      <c r="AV20">
         <v>2</v>
       </c>
       <c r="AX20">
         <v>2</v>
       </c>
       <c r="AY20">
-        <v>5</v>
-      </c>
-      <c r="BA20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="AZ20">
+        <v>5</v>
+      </c>
+      <c r="BB20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43915</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
+        <v>1087</v>
+      </c>
+      <c r="C21">
         <v>283</v>
       </c>
-      <c r="AC21">
+      <c r="AD21">
         <v>16</v>
       </c>
-      <c r="AD21">
+      <c r="AE21">
         <v>13</v>
       </c>
-      <c r="AF21">
-        <v>5</v>
-      </c>
       <c r="AG21">
+        <v>5</v>
+      </c>
+      <c r="AH21">
         <v>13</v>
       </c>
-      <c r="AH21">
+      <c r="AI21">
         <v>8</v>
       </c>
-      <c r="AI21">
+      <c r="AJ21">
         <v>6</v>
       </c>
-      <c r="AJ21">
-        <v>1</v>
-      </c>
       <c r="AK21">
         <v>1</v>
       </c>
       <c r="AL21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AM21">
+        <v>5</v>
+      </c>
+      <c r="AN21">
         <v>7</v>
       </c>
-      <c r="AN21">
-        <v>3</v>
-      </c>
       <c r="AO21">
+        <v>3</v>
+      </c>
+      <c r="AP21">
         <v>169</v>
       </c>
-      <c r="AP21">
-        <v>3</v>
-      </c>
       <c r="AQ21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AR21">
         <v>1</v>
       </c>
       <c r="AS21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AT21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AU21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AV21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AX21">
         <v>2</v>
       </c>
       <c r="AY21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AZ21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BA21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="BB21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43916</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
+        <v>1023</v>
+      </c>
+      <c r="C22">
         <v>341</v>
       </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
       <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
         <v>0</v>
       </c>
-      <c r="E22">
-        <v>3</v>
-      </c>
       <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
         <v>0</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>66</v>
       </c>
-      <c r="H22">
-        <v>5</v>
-      </c>
       <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22">
         <v>89</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>11</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>61</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>8</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>53</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>17</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>26</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>10</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>25</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <v>9</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <v>14</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>9</v>
       </c>
-      <c r="U22">
-        <v>1</v>
-      </c>
       <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
         <v>0</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>135</v>
       </c>
-      <c r="X22">
+      <c r="Y22">
         <v>207</v>
       </c>
-      <c r="Z22">
+      <c r="AA22">
         <v>69</v>
       </c>
-      <c r="AA22">
+      <c r="AB22">
         <v>31</v>
       </c>
-      <c r="AB22">
-        <v>3</v>
-      </c>
       <c r="AC22">
+        <v>3</v>
+      </c>
+      <c r="AD22">
         <v>15</v>
       </c>
-      <c r="AD22">
+      <c r="AE22">
         <v>17</v>
       </c>
-      <c r="AF22">
-        <v>5</v>
-      </c>
       <c r="AG22">
+        <v>5</v>
+      </c>
+      <c r="AH22">
         <v>19</v>
       </c>
-      <c r="AH22">
+      <c r="AI22">
         <v>12</v>
       </c>
-      <c r="AI22">
+      <c r="AJ22">
         <v>7</v>
       </c>
-      <c r="AJ22">
-        <v>1</v>
-      </c>
       <c r="AK22">
         <v>1</v>
       </c>
       <c r="AL22">
+        <v>1</v>
+      </c>
+      <c r="AM22">
         <v>6</v>
       </c>
-      <c r="AM22">
+      <c r="AN22">
         <v>8</v>
       </c>
-      <c r="AN22">
-        <v>4</v>
-      </c>
       <c r="AO22">
+        <v>4</v>
+      </c>
+      <c r="AP22">
         <v>207</v>
       </c>
-      <c r="AP22">
-        <v>3</v>
-      </c>
       <c r="AQ22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AR22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AS22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AT22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AU22">
-        <v>2</v>
-      </c>
-      <c r="AW22">
+        <v>1</v>
+      </c>
+      <c r="AV22">
         <v>2</v>
       </c>
       <c r="AX22">
         <v>2</v>
       </c>
       <c r="AY22">
-        <v>5</v>
-      </c>
-      <c r="BA22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="AZ22">
+        <v>5</v>
+      </c>
+      <c r="BB22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43917</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
+        <v>776</v>
+      </c>
+      <c r="C23">
         <v>417</v>
       </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="G23">
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="H23">
         <v>84</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>106</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>73</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>65</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>31</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>29</v>
       </c>
-      <c r="S23">
+      <c r="T23">
         <v>20</v>
       </c>
-      <c r="U23">
-        <v>2</v>
-      </c>
-      <c r="W23">
+      <c r="V23">
+        <v>2</v>
+      </c>
+      <c r="X23">
         <v>166</v>
       </c>
-      <c r="X23">
+      <c r="Y23">
         <v>249</v>
       </c>
-      <c r="Y23">
-        <v>2</v>
-      </c>
       <c r="Z23">
+        <v>2</v>
+      </c>
+      <c r="AA23">
         <v>85</v>
       </c>
-      <c r="AA23">
+      <c r="AB23">
         <v>38</v>
       </c>
-      <c r="AB23">
-        <v>5</v>
-      </c>
       <c r="AC23">
+        <v>5</v>
+      </c>
+      <c r="AD23">
         <v>18</v>
       </c>
-      <c r="AD23">
+      <c r="AE23">
         <v>21</v>
       </c>
-      <c r="AE23">
-        <v>1</v>
-      </c>
       <c r="AF23">
+        <v>1</v>
+      </c>
+      <c r="AG23">
         <v>6</v>
       </c>
-      <c r="AG23">
+      <c r="AH23">
         <v>20</v>
       </c>
-      <c r="AH23">
+      <c r="AI23">
         <v>14</v>
       </c>
-      <c r="AI23">
+      <c r="AJ23">
         <v>7</v>
       </c>
-      <c r="AJ23">
-        <v>3</v>
-      </c>
       <c r="AK23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AL23">
+        <v>1</v>
+      </c>
+      <c r="AM23">
         <v>6</v>
       </c>
-      <c r="AM23">
+      <c r="AN23">
         <v>8</v>
       </c>
-      <c r="AN23">
-        <v>5</v>
-      </c>
       <c r="AO23">
+        <v>5</v>
+      </c>
+      <c r="AP23">
         <v>251</v>
       </c>
-      <c r="AP23">
-        <v>3</v>
-      </c>
       <c r="AQ23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AR23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AS23">
+        <v>1</v>
+      </c>
+      <c r="AT23">
         <v>6</v>
       </c>
-      <c r="AT23">
-        <v>2</v>
-      </c>
       <c r="AU23">
-        <v>3</v>
-      </c>
-      <c r="AW23">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="AV23">
+        <v>3</v>
       </c>
       <c r="AX23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AY23">
+        <v>3</v>
+      </c>
+      <c r="AZ23">
         <v>6</v>
       </c>
-      <c r="BA23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43918</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>488</v>
       </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
       <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
         <v>0</v>
       </c>
-      <c r="E24">
-        <v>5</v>
-      </c>
       <c r="F24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
         <v>102</v>
       </c>
-      <c r="H24">
-        <v>5</v>
-      </c>
       <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24">
         <v>118</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>14</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>85</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>15</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>74</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>21</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>36</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <v>12</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>38</v>
       </c>
-      <c r="R24">
+      <c r="S24">
         <v>13</v>
       </c>
-      <c r="S24">
+      <c r="T24">
         <v>25</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>15</v>
       </c>
-      <c r="U24">
-        <v>2</v>
-      </c>
       <c r="V24">
+        <v>2</v>
+      </c>
+      <c r="W24">
         <v>0</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <v>206</v>
       </c>
-      <c r="X24">
+      <c r="Y24">
         <v>280</v>
       </c>
-      <c r="Y24">
-        <v>2</v>
-      </c>
       <c r="Z24">
+        <v>2</v>
+      </c>
+      <c r="AA24">
         <v>96</v>
       </c>
-      <c r="AA24">
+      <c r="AB24">
         <v>42</v>
       </c>
-      <c r="AB24">
+      <c r="AC24">
         <v>7</v>
       </c>
-      <c r="AC24">
+      <c r="AD24">
         <v>19</v>
       </c>
-      <c r="AD24">
+      <c r="AE24">
         <v>24</v>
       </c>
-      <c r="AE24">
-        <v>1</v>
-      </c>
       <c r="AF24">
+        <v>1</v>
+      </c>
+      <c r="AG24">
         <v>6</v>
       </c>
-      <c r="AG24">
+      <c r="AH24">
         <v>26</v>
       </c>
-      <c r="AH24">
+      <c r="AI24">
         <v>16</v>
       </c>
-      <c r="AI24">
+      <c r="AJ24">
         <v>9</v>
       </c>
-      <c r="AJ24">
-        <v>3</v>
-      </c>
       <c r="AK24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL24">
+        <v>2</v>
+      </c>
+      <c r="AM24">
         <v>8</v>
       </c>
-      <c r="AM24">
+      <c r="AN24">
         <v>11</v>
       </c>
-      <c r="AN24">
+      <c r="AO24">
         <v>7</v>
       </c>
-      <c r="AO24">
+      <c r="AP24">
         <v>284</v>
       </c>
-      <c r="AP24">
-        <v>3</v>
-      </c>
       <c r="AQ24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AR24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AS24">
+        <v>1</v>
+      </c>
+      <c r="AT24">
         <v>10</v>
       </c>
-      <c r="AT24">
-        <v>2</v>
-      </c>
       <c r="AU24">
-        <v>4</v>
-      </c>
-      <c r="AW24">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="AV24">
+        <v>4</v>
       </c>
       <c r="AX24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AY24">
+        <v>4</v>
+      </c>
+      <c r="AZ24">
         <v>7</v>
       </c>
-      <c r="BA24">
+      <c r="BB24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>43919</v>
+      </c>
+      <c r="C25">
+        <v>519</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="H25">
+        <v>107</v>
+      </c>
+      <c r="J25">
+        <v>130</v>
+      </c>
+      <c r="L25">
+        <v>90</v>
+      </c>
+      <c r="N25">
+        <v>79</v>
+      </c>
+      <c r="P25">
+        <v>37</v>
+      </c>
+      <c r="R25">
+        <v>39</v>
+      </c>
+      <c r="T25">
+        <v>26</v>
+      </c>
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <v>219</v>
+      </c>
+      <c r="Y25">
+        <v>298</v>
+      </c>
+      <c r="Z25">
+        <v>2</v>
+      </c>
+      <c r="AA25">
+        <v>106</v>
+      </c>
+      <c r="AB25">
+        <v>47</v>
+      </c>
+      <c r="AC25">
+        <v>7</v>
+      </c>
+      <c r="AD25">
+        <v>20</v>
+      </c>
+      <c r="AE25">
+        <v>24</v>
+      </c>
+      <c r="AF25">
+        <v>1</v>
+      </c>
+      <c r="AG25">
+        <v>6</v>
+      </c>
+      <c r="AH25">
+        <v>29</v>
+      </c>
+      <c r="AI25">
+        <v>18</v>
+      </c>
+      <c r="AJ25">
+        <v>9</v>
+      </c>
+      <c r="AK25">
+        <v>4</v>
+      </c>
+      <c r="AL25">
+        <v>3</v>
+      </c>
+      <c r="AM25">
+        <v>8</v>
+      </c>
+      <c r="AN25">
+        <v>11</v>
+      </c>
+      <c r="AO25">
+        <v>7</v>
+      </c>
+      <c r="AP25">
+        <v>314</v>
+      </c>
+      <c r="AQ25">
+        <v>4</v>
+      </c>
+      <c r="AR25">
+        <v>2</v>
+      </c>
+      <c r="AS25">
+        <v>2</v>
+      </c>
+      <c r="AT25">
+        <v>10</v>
+      </c>
+      <c r="AU25">
+        <v>2</v>
+      </c>
+      <c r="AV25">
+        <v>4</v>
+      </c>
+      <c r="AX25">
+        <v>3</v>
+      </c>
+      <c r="AY25">
+        <v>4</v>
+      </c>
+      <c r="AZ25">
+        <v>7</v>
+      </c>
+      <c r="BB25">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added data from Mar 30
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA98C8F6-0927-B448-9541-66DB4B518C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03638F70-B2F1-9D49-AD56-8F8EDDCA068B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="7740" yWindow="460" windowWidth="14200" windowHeight="17540" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -545,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BB25"/>
+  <dimension ref="A1:BB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BD25" sqref="BD25"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BC26" sqref="BC26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1507,6 +1507,9 @@
       <c r="A24" s="1">
         <v>43918</v>
       </c>
+      <c r="B24" s="2">
+        <v>1275</v>
+      </c>
       <c r="C24">
         <v>488</v>
       </c>
@@ -1781,6 +1784,161 @@
       </c>
       <c r="BB25">
         <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>43920</v>
+      </c>
+      <c r="C26">
+        <v>603</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>121</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="J26">
+        <v>148</v>
+      </c>
+      <c r="K26">
+        <v>17</v>
+      </c>
+      <c r="L26">
+        <v>105</v>
+      </c>
+      <c r="M26">
+        <v>17</v>
+      </c>
+      <c r="N26">
+        <v>91</v>
+      </c>
+      <c r="O26">
+        <v>25</v>
+      </c>
+      <c r="P26">
+        <v>52</v>
+      </c>
+      <c r="Q26">
+        <v>15</v>
+      </c>
+      <c r="R26">
+        <v>45</v>
+      </c>
+      <c r="S26">
+        <v>17</v>
+      </c>
+      <c r="T26">
+        <v>29</v>
+      </c>
+      <c r="U26">
+        <v>20</v>
+      </c>
+      <c r="V26">
+        <v>2</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>256</v>
+      </c>
+      <c r="Y26">
+        <v>345</v>
+      </c>
+      <c r="Z26">
+        <v>2</v>
+      </c>
+      <c r="AA26">
+        <v>118</v>
+      </c>
+      <c r="AB26">
+        <v>51</v>
+      </c>
+      <c r="AC26">
+        <v>7</v>
+      </c>
+      <c r="AD26">
+        <v>24</v>
+      </c>
+      <c r="AE26">
+        <v>32</v>
+      </c>
+      <c r="AF26">
+        <v>1</v>
+      </c>
+      <c r="AG26">
+        <v>6</v>
+      </c>
+      <c r="AH26">
+        <v>34</v>
+      </c>
+      <c r="AI26">
+        <v>19</v>
+      </c>
+      <c r="AJ26">
+        <v>10</v>
+      </c>
+      <c r="AK26">
+        <v>6</v>
+      </c>
+      <c r="AL26">
+        <v>4</v>
+      </c>
+      <c r="AM26">
+        <v>8</v>
+      </c>
+      <c r="AN26">
+        <v>14</v>
+      </c>
+      <c r="AO26">
+        <v>7</v>
+      </c>
+      <c r="AP26">
+        <v>350</v>
+      </c>
+      <c r="AQ26">
+        <v>5</v>
+      </c>
+      <c r="AR26">
+        <v>3</v>
+      </c>
+      <c r="AS26">
+        <v>2</v>
+      </c>
+      <c r="AT26">
+        <v>11</v>
+      </c>
+      <c r="AU26">
+        <v>4</v>
+      </c>
+      <c r="AV26">
+        <v>4</v>
+      </c>
+      <c r="AX26">
+        <v>4</v>
+      </c>
+      <c r="AY26">
+        <v>4</v>
+      </c>
+      <c r="AZ26">
+        <v>10</v>
+      </c>
+      <c r="BB26">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated w Mar 31 data
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03638F70-B2F1-9D49-AD56-8F8EDDCA068B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC485B78-C408-E74B-B6F6-3521C943254C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="460" windowWidth="14200" windowHeight="17540" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-31020" yWindow="-2900" windowWidth="14200" windowHeight="17540" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AZ$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BA$17</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>date</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>tested</t>
+  </si>
+  <si>
+    <t>imperialbeach</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -545,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BB26"/>
+  <dimension ref="A1:BD27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="BC26" sqref="BC26"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,11 +562,11 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="10.83203125" style="2"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.83203125" customWidth="1"/>
+    <col min="53" max="53" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -670,71 +676,77 @@
         <v>23</v>
       </c>
       <c r="AK1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>39</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>24</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>25</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>26</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>27</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>28</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>30</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>31</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>37</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>32</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>40</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>36</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>33</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>34</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>41</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="BD1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43896</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43897</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
@@ -742,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
@@ -750,7 +762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43900</v>
       </c>
@@ -758,7 +770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43901</v>
       </c>
@@ -766,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
@@ -774,7 +786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43903</v>
       </c>
@@ -785,7 +797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43904</v>
       </c>
@@ -796,7 +808,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43905</v>
       </c>
@@ -807,7 +819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43906</v>
       </c>
@@ -818,7 +830,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43907</v>
       </c>
@@ -829,7 +841,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43908</v>
       </c>
@@ -840,7 +852,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43909</v>
       </c>
@@ -851,7 +863,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43910</v>
       </c>
@@ -862,7 +874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43911</v>
       </c>
@@ -890,41 +902,41 @@
       <c r="AJ17">
         <v>2</v>
       </c>
-      <c r="AM17">
-        <v>1</v>
-      </c>
       <c r="AN17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AO17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AP17">
+        <v>1</v>
+      </c>
+      <c r="AQ17">
         <v>87</v>
       </c>
-      <c r="AQ17">
-        <v>3</v>
-      </c>
       <c r="AR17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AS17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT17">
         <v>2</v>
       </c>
-      <c r="AV17">
-        <v>2</v>
-      </c>
-      <c r="AY17">
+      <c r="AU17">
+        <v>2</v>
+      </c>
+      <c r="AW17">
         <v>2</v>
       </c>
       <c r="AZ17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="BA17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43912</v>
       </c>
@@ -952,47 +964,47 @@
       <c r="AJ18">
         <v>3</v>
       </c>
-      <c r="AK18">
-        <v>1</v>
-      </c>
-      <c r="AM18">
-        <v>2</v>
+      <c r="AL18">
+        <v>1</v>
       </c>
       <c r="AN18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AO18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AP18">
+        <v>2</v>
+      </c>
+      <c r="AQ18">
         <v>118</v>
       </c>
-      <c r="AQ18">
-        <v>3</v>
-      </c>
       <c r="AR18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AS18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT18">
         <v>2</v>
       </c>
-      <c r="AV18">
-        <v>2</v>
-      </c>
-      <c r="AX18">
-        <v>1</v>
+      <c r="AU18">
+        <v>2</v>
+      </c>
+      <c r="AW18">
+        <v>2</v>
       </c>
       <c r="AY18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:54" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="BA18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43913</v>
       </c>
@@ -1020,53 +1032,53 @@
       <c r="AJ19">
         <v>5</v>
       </c>
-      <c r="AK19">
-        <v>1</v>
-      </c>
-      <c r="AM19">
-        <v>3</v>
+      <c r="AL19">
+        <v>1</v>
       </c>
       <c r="AN19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AO19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AP19">
+        <v>2</v>
+      </c>
+      <c r="AQ19">
         <v>134</v>
       </c>
-      <c r="AQ19">
-        <v>3</v>
-      </c>
       <c r="AR19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AS19">
         <v>1</v>
       </c>
       <c r="AT19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AU19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AV19">
-        <v>2</v>
-      </c>
-      <c r="AX19">
+        <v>1</v>
+      </c>
+      <c r="AW19">
         <v>2</v>
       </c>
       <c r="AY19">
         <v>2</v>
       </c>
       <c r="AZ19">
-        <v>5</v>
-      </c>
-      <c r="BB19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:54" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="BA19">
+        <v>5</v>
+      </c>
+      <c r="BC19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43914</v>
       </c>
@@ -1094,53 +1106,53 @@
       <c r="AJ20">
         <v>6</v>
       </c>
-      <c r="AK20">
-        <v>1</v>
-      </c>
-      <c r="AM20">
-        <v>3</v>
+      <c r="AL20">
+        <v>1</v>
       </c>
       <c r="AN20">
+        <v>3</v>
+      </c>
+      <c r="AO20">
         <v>7</v>
       </c>
-      <c r="AO20">
-        <v>2</v>
-      </c>
       <c r="AP20">
+        <v>2</v>
+      </c>
+      <c r="AQ20">
         <v>141</v>
       </c>
-      <c r="AQ20">
-        <v>3</v>
-      </c>
       <c r="AR20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AS20">
         <v>1</v>
       </c>
       <c r="AT20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AU20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AV20">
-        <v>2</v>
-      </c>
-      <c r="AX20">
+        <v>1</v>
+      </c>
+      <c r="AW20">
         <v>2</v>
       </c>
       <c r="AY20">
         <v>2</v>
       </c>
       <c r="AZ20">
-        <v>5</v>
-      </c>
-      <c r="BB20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:54" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="BA20">
+        <v>5</v>
+      </c>
+      <c r="BC20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43915</v>
       </c>
@@ -1168,62 +1180,62 @@
       <c r="AJ21">
         <v>6</v>
       </c>
-      <c r="AK21">
-        <v>1</v>
-      </c>
       <c r="AL21">
         <v>1</v>
       </c>
       <c r="AM21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AN21">
+        <v>5</v>
+      </c>
+      <c r="AO21">
         <v>7</v>
       </c>
-      <c r="AO21">
-        <v>3</v>
-      </c>
       <c r="AP21">
+        <v>3</v>
+      </c>
+      <c r="AQ21">
         <v>169</v>
       </c>
-      <c r="AQ21">
-        <v>3</v>
-      </c>
       <c r="AR21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AS21">
         <v>1</v>
       </c>
       <c r="AT21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AU21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AV21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AY21">
         <v>2</v>
       </c>
       <c r="AZ21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BA21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BB21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:54" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="BC21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43916</v>
       </c>
@@ -1326,56 +1338,56 @@
       <c r="AJ22">
         <v>7</v>
       </c>
-      <c r="AK22">
-        <v>1</v>
-      </c>
       <c r="AL22">
         <v>1</v>
       </c>
       <c r="AM22">
+        <v>1</v>
+      </c>
+      <c r="AN22">
         <v>6</v>
       </c>
-      <c r="AN22">
+      <c r="AO22">
         <v>8</v>
       </c>
-      <c r="AO22">
-        <v>4</v>
-      </c>
       <c r="AP22">
+        <v>4</v>
+      </c>
+      <c r="AQ22">
         <v>207</v>
       </c>
-      <c r="AQ22">
-        <v>3</v>
-      </c>
       <c r="AR22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AS22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AU22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AV22">
-        <v>2</v>
-      </c>
-      <c r="AX22">
+        <v>1</v>
+      </c>
+      <c r="AW22">
         <v>2</v>
       </c>
       <c r="AY22">
         <v>2</v>
       </c>
       <c r="AZ22">
-        <v>5</v>
-      </c>
-      <c r="BB22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:54" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="BA22">
+        <v>5</v>
+      </c>
+      <c r="BC22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43917</v>
       </c>
@@ -1454,56 +1466,56 @@
       <c r="AJ23">
         <v>7</v>
       </c>
-      <c r="AK23">
-        <v>3</v>
-      </c>
       <c r="AL23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AM23">
+        <v>1</v>
+      </c>
+      <c r="AN23">
         <v>6</v>
       </c>
-      <c r="AN23">
+      <c r="AO23">
         <v>8</v>
       </c>
-      <c r="AO23">
-        <v>5</v>
-      </c>
       <c r="AP23">
+        <v>5</v>
+      </c>
+      <c r="AQ23">
         <v>251</v>
       </c>
-      <c r="AQ23">
-        <v>3</v>
-      </c>
       <c r="AR23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AS23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT23">
+        <v>1</v>
+      </c>
+      <c r="AU23">
         <v>6</v>
       </c>
-      <c r="AU23">
-        <v>2</v>
-      </c>
       <c r="AV23">
-        <v>3</v>
-      </c>
-      <c r="AX23">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="AW23">
+        <v>3</v>
       </c>
       <c r="AY23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AZ23">
+        <v>3</v>
+      </c>
+      <c r="BA23">
         <v>6</v>
       </c>
-      <c r="BB23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="BC23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43918</v>
       </c>
@@ -1612,59 +1624,62 @@
       <c r="AJ24">
         <v>9</v>
       </c>
-      <c r="AK24">
-        <v>3</v>
-      </c>
       <c r="AL24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AM24">
+        <v>2</v>
+      </c>
+      <c r="AN24">
         <v>8</v>
       </c>
-      <c r="AN24">
+      <c r="AO24">
         <v>11</v>
       </c>
-      <c r="AO24">
+      <c r="AP24">
         <v>7</v>
       </c>
-      <c r="AP24">
+      <c r="AQ24">
         <v>284</v>
       </c>
-      <c r="AQ24">
-        <v>3</v>
-      </c>
       <c r="AR24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AS24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT24">
+        <v>1</v>
+      </c>
+      <c r="AU24">
         <v>10</v>
       </c>
-      <c r="AU24">
-        <v>2</v>
-      </c>
       <c r="AV24">
-        <v>4</v>
-      </c>
-      <c r="AX24">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="AW24">
+        <v>4</v>
       </c>
       <c r="AY24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AZ24">
+        <v>4</v>
+      </c>
+      <c r="BA24">
         <v>7</v>
       </c>
-      <c r="BB24">
+      <c r="BC24">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43919</v>
       </c>
+      <c r="B25" s="2">
+        <v>687</v>
+      </c>
       <c r="C25">
         <v>519</v>
       </c>
@@ -1737,59 +1752,62 @@
       <c r="AJ25">
         <v>9</v>
       </c>
-      <c r="AK25">
-        <v>4</v>
-      </c>
       <c r="AL25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AM25">
+        <v>3</v>
+      </c>
+      <c r="AN25">
         <v>8</v>
       </c>
-      <c r="AN25">
+      <c r="AO25">
         <v>11</v>
       </c>
-      <c r="AO25">
+      <c r="AP25">
         <v>7</v>
       </c>
-      <c r="AP25">
+      <c r="AQ25">
         <v>314</v>
       </c>
-      <c r="AQ25">
-        <v>4</v>
-      </c>
       <c r="AR25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AS25">
         <v>2</v>
       </c>
       <c r="AT25">
+        <v>2</v>
+      </c>
+      <c r="AU25">
         <v>10</v>
       </c>
-      <c r="AU25">
-        <v>2</v>
-      </c>
       <c r="AV25">
-        <v>4</v>
-      </c>
-      <c r="AX25">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="AW25">
+        <v>4</v>
       </c>
       <c r="AY25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AZ25">
+        <v>4</v>
+      </c>
+      <c r="BA25">
         <v>7</v>
       </c>
-      <c r="BB25">
+      <c r="BC25">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43920</v>
       </c>
+      <c r="B26" s="2">
+        <v>1538</v>
+      </c>
       <c r="C26">
         <v>603</v>
       </c>
@@ -1892,53 +1910,208 @@
       <c r="AJ26">
         <v>10</v>
       </c>
-      <c r="AK26">
+      <c r="AL26">
         <v>6</v>
       </c>
-      <c r="AL26">
-        <v>4</v>
-      </c>
       <c r="AM26">
+        <v>4</v>
+      </c>
+      <c r="AN26">
         <v>8</v>
       </c>
-      <c r="AN26">
+      <c r="AO26">
         <v>14</v>
       </c>
-      <c r="AO26">
+      <c r="AP26">
         <v>7</v>
       </c>
-      <c r="AP26">
+      <c r="AQ26">
         <v>350</v>
       </c>
-      <c r="AQ26">
-        <v>5</v>
-      </c>
       <c r="AR26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AS26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AT26">
+        <v>2</v>
+      </c>
+      <c r="AU26">
         <v>11</v>
       </c>
-      <c r="AU26">
-        <v>4</v>
-      </c>
       <c r="AV26">
         <v>4</v>
       </c>
-      <c r="AX26">
+      <c r="AW26">
         <v>4</v>
       </c>
       <c r="AY26">
         <v>4</v>
       </c>
       <c r="AZ26">
+        <v>4</v>
+      </c>
+      <c r="BA26">
         <v>10</v>
       </c>
-      <c r="BB26">
+      <c r="BC26">
         <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>43921</v>
+      </c>
+      <c r="C27">
+        <v>734</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>144</v>
+      </c>
+      <c r="I27">
+        <v>8</v>
+      </c>
+      <c r="J27">
+        <v>174</v>
+      </c>
+      <c r="K27">
+        <v>17</v>
+      </c>
+      <c r="L27">
+        <v>130</v>
+      </c>
+      <c r="M27">
+        <v>18</v>
+      </c>
+      <c r="N27">
+        <v>116</v>
+      </c>
+      <c r="O27">
+        <v>27</v>
+      </c>
+      <c r="P27">
+        <v>74</v>
+      </c>
+      <c r="Q27">
+        <v>20</v>
+      </c>
+      <c r="R27">
+        <v>49</v>
+      </c>
+      <c r="S27">
+        <v>22</v>
+      </c>
+      <c r="T27">
+        <v>34</v>
+      </c>
+      <c r="U27">
+        <v>23</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>317</v>
+      </c>
+      <c r="Y27">
+        <v>414</v>
+      </c>
+      <c r="Z27">
+        <v>3</v>
+      </c>
+      <c r="AA27">
+        <v>136</v>
+      </c>
+      <c r="AB27">
+        <v>56</v>
+      </c>
+      <c r="AC27">
+        <v>9</v>
+      </c>
+      <c r="AD27">
+        <v>27</v>
+      </c>
+      <c r="AE27">
+        <v>38</v>
+      </c>
+      <c r="AF27">
+        <v>1</v>
+      </c>
+      <c r="AG27">
+        <v>5</v>
+      </c>
+      <c r="AH27">
+        <v>36</v>
+      </c>
+      <c r="AI27">
+        <v>20</v>
+      </c>
+      <c r="AJ27">
+        <v>11</v>
+      </c>
+      <c r="AL27">
+        <v>8</v>
+      </c>
+      <c r="AM27">
+        <v>5</v>
+      </c>
+      <c r="AN27">
+        <v>10</v>
+      </c>
+      <c r="AO27">
+        <v>17</v>
+      </c>
+      <c r="AP27">
+        <v>7</v>
+      </c>
+      <c r="AQ27">
+        <v>422</v>
+      </c>
+      <c r="AR27">
+        <v>5</v>
+      </c>
+      <c r="AS27">
+        <v>5</v>
+      </c>
+      <c r="AT27">
+        <v>3</v>
+      </c>
+      <c r="AU27">
+        <v>8</v>
+      </c>
+      <c r="AV27">
+        <v>3</v>
+      </c>
+      <c r="AW27">
+        <v>4</v>
+      </c>
+      <c r="AY27">
+        <v>5</v>
+      </c>
+      <c r="AZ27">
+        <v>4</v>
+      </c>
+      <c r="BA27">
+        <v>11</v>
+      </c>
+      <c r="BC27">
+        <v>17</v>
+      </c>
+      <c r="BD27">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated w Apr 1 Data
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC485B78-C408-E74B-B6F6-3521C943254C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0BDFE1-3554-9944-8F24-6C2274DA1A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31020" yWindow="-2900" windowWidth="14200" windowHeight="17540" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-33920" yWindow="-3140" windowWidth="27380" windowHeight="16060" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BA$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BB$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>date</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>paumavalley</t>
   </si>
 </sst>
 </file>
@@ -551,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BD27"/>
+  <dimension ref="A1:BE28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,11 +565,11 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="10.83203125" style="2"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.83203125" customWidth="1"/>
+    <col min="54" max="54" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,32 +724,35 @@
         <v>36</v>
       </c>
       <c r="AZ1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BA1" t="s">
         <v>33</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>34</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>41</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>38</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43896</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43897</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
@@ -754,7 +760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
@@ -762,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43900</v>
       </c>
@@ -770,7 +776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43901</v>
       </c>
@@ -778,7 +784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
@@ -786,7 +792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43903</v>
       </c>
@@ -797,7 +803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43904</v>
       </c>
@@ -808,7 +814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43905</v>
       </c>
@@ -819,7 +825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43906</v>
       </c>
@@ -830,7 +836,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43907</v>
       </c>
@@ -841,7 +847,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43908</v>
       </c>
@@ -852,7 +858,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43909</v>
       </c>
@@ -863,7 +869,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43910</v>
       </c>
@@ -874,7 +880,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43911</v>
       </c>
@@ -929,14 +935,14 @@
       <c r="AW17">
         <v>2</v>
       </c>
-      <c r="AZ17">
-        <v>2</v>
-      </c>
       <c r="BA17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BB17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43912</v>
       </c>
@@ -997,14 +1003,14 @@
       <c r="AY18">
         <v>1</v>
       </c>
-      <c r="AZ18">
-        <v>2</v>
-      </c>
       <c r="BA18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="BB18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43913</v>
       </c>
@@ -1068,17 +1074,17 @@
       <c r="AY19">
         <v>2</v>
       </c>
-      <c r="AZ19">
-        <v>2</v>
-      </c>
       <c r="BA19">
-        <v>5</v>
-      </c>
-      <c r="BC19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="BB19">
+        <v>5</v>
+      </c>
+      <c r="BD19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43914</v>
       </c>
@@ -1142,17 +1148,17 @@
       <c r="AY20">
         <v>2</v>
       </c>
-      <c r="AZ20">
-        <v>2</v>
-      </c>
       <c r="BA20">
-        <v>5</v>
-      </c>
-      <c r="BC20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="BB20">
+        <v>5</v>
+      </c>
+      <c r="BD20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43915</v>
       </c>
@@ -1222,20 +1228,20 @@
       <c r="AY21">
         <v>2</v>
       </c>
-      <c r="AZ21">
-        <v>2</v>
-      </c>
       <c r="BA21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BB21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BC21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="BD21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43916</v>
       </c>
@@ -1377,17 +1383,17 @@
       <c r="AY22">
         <v>2</v>
       </c>
-      <c r="AZ22">
-        <v>2</v>
-      </c>
       <c r="BA22">
-        <v>5</v>
-      </c>
-      <c r="BC22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="BB22">
+        <v>5</v>
+      </c>
+      <c r="BD22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43917</v>
       </c>
@@ -1505,17 +1511,17 @@
       <c r="AY23">
         <v>2</v>
       </c>
-      <c r="AZ23">
-        <v>3</v>
-      </c>
       <c r="BA23">
+        <v>3</v>
+      </c>
+      <c r="BB23">
         <v>6</v>
       </c>
-      <c r="BC23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BD23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43918</v>
       </c>
@@ -1663,17 +1669,17 @@
       <c r="AY24">
         <v>2</v>
       </c>
-      <c r="AZ24">
-        <v>4</v>
-      </c>
       <c r="BA24">
+        <v>4</v>
+      </c>
+      <c r="BB24">
         <v>7</v>
       </c>
-      <c r="BC24">
+      <c r="BD24">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43919</v>
       </c>
@@ -1791,17 +1797,17 @@
       <c r="AY25">
         <v>3</v>
       </c>
-      <c r="AZ25">
-        <v>4</v>
-      </c>
       <c r="BA25">
+        <v>4</v>
+      </c>
+      <c r="BB25">
         <v>7</v>
       </c>
-      <c r="BC25">
+      <c r="BD25">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43920</v>
       </c>
@@ -1949,20 +1955,23 @@
       <c r="AY26">
         <v>4</v>
       </c>
-      <c r="AZ26">
-        <v>4</v>
-      </c>
       <c r="BA26">
+        <v>4</v>
+      </c>
+      <c r="BB26">
         <v>10</v>
       </c>
-      <c r="BC26">
+      <c r="BD26">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43921</v>
       </c>
+      <c r="B27" s="2">
+        <v>989</v>
+      </c>
       <c r="C27">
         <v>734</v>
       </c>
@@ -2101,17 +2110,178 @@
       <c r="AY27">
         <v>5</v>
       </c>
-      <c r="AZ27">
-        <v>4</v>
-      </c>
       <c r="BA27">
+        <v>4</v>
+      </c>
+      <c r="BB27">
         <v>11</v>
       </c>
-      <c r="BC27">
+      <c r="BD27">
         <v>17</v>
       </c>
-      <c r="BD27">
+      <c r="BE27">
         <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>43922</v>
+      </c>
+      <c r="C28">
+        <v>849</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>163</v>
+      </c>
+      <c r="I28">
+        <v>10</v>
+      </c>
+      <c r="J28">
+        <v>194</v>
+      </c>
+      <c r="K28">
+        <v>18</v>
+      </c>
+      <c r="L28">
+        <v>154</v>
+      </c>
+      <c r="M28">
+        <v>19</v>
+      </c>
+      <c r="N28">
+        <v>125</v>
+      </c>
+      <c r="O28">
+        <v>31</v>
+      </c>
+      <c r="P28">
+        <v>93</v>
+      </c>
+      <c r="Q28">
+        <v>27</v>
+      </c>
+      <c r="R28">
+        <v>62</v>
+      </c>
+      <c r="S28">
+        <v>27</v>
+      </c>
+      <c r="T28">
+        <v>41</v>
+      </c>
+      <c r="U28">
+        <v>25</v>
+      </c>
+      <c r="V28">
+        <v>3</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>380</v>
+      </c>
+      <c r="Y28">
+        <v>461</v>
+      </c>
+      <c r="Z28">
+        <v>8</v>
+      </c>
+      <c r="AA28">
+        <v>158</v>
+      </c>
+      <c r="AB28">
+        <v>65</v>
+      </c>
+      <c r="AC28">
+        <v>15</v>
+      </c>
+      <c r="AD28">
+        <v>30</v>
+      </c>
+      <c r="AE28">
+        <v>52</v>
+      </c>
+      <c r="AF28">
+        <v>2</v>
+      </c>
+      <c r="AG28">
+        <v>5</v>
+      </c>
+      <c r="AH28">
+        <v>38</v>
+      </c>
+      <c r="AI28">
+        <v>24</v>
+      </c>
+      <c r="AJ28">
+        <v>14</v>
+      </c>
+      <c r="AL28">
+        <v>11</v>
+      </c>
+      <c r="AM28">
+        <v>5</v>
+      </c>
+      <c r="AN28">
+        <v>11</v>
+      </c>
+      <c r="AO28">
+        <v>20</v>
+      </c>
+      <c r="AP28">
+        <v>9</v>
+      </c>
+      <c r="AQ28">
+        <v>486</v>
+      </c>
+      <c r="AR28">
+        <v>10</v>
+      </c>
+      <c r="AS28">
+        <v>5</v>
+      </c>
+      <c r="AT28">
+        <v>3</v>
+      </c>
+      <c r="AU28">
+        <v>9</v>
+      </c>
+      <c r="AV28">
+        <v>6</v>
+      </c>
+      <c r="AW28">
+        <v>4</v>
+      </c>
+      <c r="AY28">
+        <v>8</v>
+      </c>
+      <c r="AZ28">
+        <v>1</v>
+      </c>
+      <c r="BA28">
+        <v>4</v>
+      </c>
+      <c r="BB28">
+        <v>12</v>
+      </c>
+      <c r="BD28">
+        <v>18</v>
+      </c>
+      <c r="BE28">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with Apr 2 data
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0BDFE1-3554-9944-8F24-6C2274DA1A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992D6764-81AE-2544-819D-97FE70ECD808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33920" yWindow="-3140" windowWidth="27380" windowHeight="16060" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="440" yWindow="1380" windowWidth="27380" windowHeight="16060" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -554,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BE28"/>
+  <dimension ref="A1:BE29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+    <sheetView tabSelected="1" topLeftCell="O4" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2127,6 +2127,9 @@
       <c r="A28" s="1">
         <v>43922</v>
       </c>
+      <c r="B28" s="2">
+        <v>2607</v>
+      </c>
       <c r="C28">
         <v>849</v>
       </c>
@@ -2282,6 +2285,170 @@
       </c>
       <c r="BE28">
         <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>43923</v>
+      </c>
+      <c r="C29">
+        <v>966</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>187</v>
+      </c>
+      <c r="I29">
+        <v>10</v>
+      </c>
+      <c r="J29">
+        <v>216</v>
+      </c>
+      <c r="K29">
+        <v>23</v>
+      </c>
+      <c r="L29">
+        <v>170</v>
+      </c>
+      <c r="M29">
+        <v>24</v>
+      </c>
+      <c r="N29">
+        <v>149</v>
+      </c>
+      <c r="O29">
+        <v>34</v>
+      </c>
+      <c r="P29">
+        <v>108</v>
+      </c>
+      <c r="Q29">
+        <v>32</v>
+      </c>
+      <c r="R29">
+        <v>71</v>
+      </c>
+      <c r="S29">
+        <v>27</v>
+      </c>
+      <c r="T29">
+        <v>45</v>
+      </c>
+      <c r="U29">
+        <v>29</v>
+      </c>
+      <c r="V29">
+        <v>3</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>439</v>
+      </c>
+      <c r="Y29">
+        <v>514</v>
+      </c>
+      <c r="Z29">
+        <v>13</v>
+      </c>
+      <c r="AA29">
+        <v>181</v>
+      </c>
+      <c r="AB29">
+        <v>70</v>
+      </c>
+      <c r="AC29">
+        <v>16</v>
+      </c>
+      <c r="AD29">
+        <v>32</v>
+      </c>
+      <c r="AE29">
+        <v>65</v>
+      </c>
+      <c r="AF29">
+        <v>2</v>
+      </c>
+      <c r="AG29">
+        <v>5</v>
+      </c>
+      <c r="AH29">
+        <v>43</v>
+      </c>
+      <c r="AI29">
+        <v>25</v>
+      </c>
+      <c r="AJ29">
+        <v>23</v>
+      </c>
+      <c r="AK29">
+        <v>1</v>
+      </c>
+      <c r="AL29">
+        <v>12</v>
+      </c>
+      <c r="AM29">
+        <v>8</v>
+      </c>
+      <c r="AN29">
+        <v>12</v>
+      </c>
+      <c r="AO29">
+        <v>22</v>
+      </c>
+      <c r="AP29">
+        <v>10</v>
+      </c>
+      <c r="AQ29">
+        <v>540</v>
+      </c>
+      <c r="AR29">
+        <v>12</v>
+      </c>
+      <c r="AS29">
+        <v>10</v>
+      </c>
+      <c r="AT29">
+        <v>5</v>
+      </c>
+      <c r="AU29">
+        <v>9</v>
+      </c>
+      <c r="AV29">
+        <v>6</v>
+      </c>
+      <c r="AW29">
+        <v>6</v>
+      </c>
+      <c r="AY29">
+        <v>8</v>
+      </c>
+      <c r="AZ29">
+        <v>2</v>
+      </c>
+      <c r="BA29">
+        <v>4</v>
+      </c>
+      <c r="BB29">
+        <v>14</v>
+      </c>
+      <c r="BD29">
+        <v>21</v>
+      </c>
+      <c r="BE29">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data from Apr 3
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992D6764-81AE-2544-819D-97FE70ECD808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADA7FD2-1CEE-1946-A846-9831B68DFEB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="1380" windowWidth="27380" windowHeight="16060" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BB$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BE$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>date</t>
   </si>
@@ -201,6 +201,18 @@
   </si>
   <si>
     <t>paumavalley</t>
+  </si>
+  <si>
+    <t>alpine</t>
+  </si>
+  <si>
+    <t>borregosprings</t>
+  </si>
+  <si>
+    <t>descando</t>
+  </si>
+  <si>
+    <t>valleycenter</t>
   </si>
 </sst>
 </file>
@@ -554,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BE29"/>
+  <dimension ref="A1:BI30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O4" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Y30" sqref="Y30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,11 +577,13 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="10.83203125" style="2"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.83203125" customWidth="1"/>
+    <col min="50" max="50" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.33203125" customWidth="1"/>
+    <col min="57" max="57" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,47 +726,59 @@
         <v>31</v>
       </c>
       <c r="AV1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AW1" t="s">
         <v>37</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>32</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>40</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>36</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>54</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>33</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BE1" t="s">
         <v>34</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>41</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>38</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43896</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43897</v>
       </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
@@ -760,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
@@ -768,7 +794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43900</v>
       </c>
@@ -776,7 +802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43901</v>
       </c>
@@ -784,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
@@ -792,7 +818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43903</v>
       </c>
@@ -803,7 +829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43904</v>
       </c>
@@ -814,7 +840,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43905</v>
       </c>
@@ -825,7 +851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43906</v>
       </c>
@@ -836,7 +862,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43907</v>
       </c>
@@ -847,7 +873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43908</v>
       </c>
@@ -858,7 +884,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43909</v>
       </c>
@@ -869,7 +895,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43910</v>
       </c>
@@ -880,7 +906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43911</v>
       </c>
@@ -932,17 +958,17 @@
       <c r="AU17">
         <v>2</v>
       </c>
-      <c r="AW17">
-        <v>2</v>
-      </c>
-      <c r="BA17">
-        <v>2</v>
-      </c>
-      <c r="BB17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="AZ17">
+        <v>2</v>
+      </c>
+      <c r="BD17">
+        <v>2</v>
+      </c>
+      <c r="BE17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43912</v>
       </c>
@@ -997,20 +1023,20 @@
       <c r="AU18">
         <v>2</v>
       </c>
-      <c r="AW18">
-        <v>2</v>
-      </c>
-      <c r="AY18">
-        <v>1</v>
-      </c>
-      <c r="BA18">
+      <c r="AZ18">
         <v>2</v>
       </c>
       <c r="BB18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="BD18">
+        <v>2</v>
+      </c>
+      <c r="BE18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43913</v>
       </c>
@@ -1065,26 +1091,26 @@
       <c r="AU19">
         <v>2</v>
       </c>
-      <c r="AV19">
-        <v>1</v>
-      </c>
       <c r="AW19">
-        <v>2</v>
-      </c>
-      <c r="AY19">
-        <v>2</v>
-      </c>
-      <c r="BA19">
+        <v>1</v>
+      </c>
+      <c r="AZ19">
         <v>2</v>
       </c>
       <c r="BB19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BD19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BE19">
+        <v>5</v>
+      </c>
+      <c r="BG19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43914</v>
       </c>
@@ -1139,26 +1165,26 @@
       <c r="AU20">
         <v>2</v>
       </c>
-      <c r="AV20">
-        <v>1</v>
-      </c>
       <c r="AW20">
-        <v>2</v>
-      </c>
-      <c r="AY20">
-        <v>2</v>
-      </c>
-      <c r="BA20">
+        <v>1</v>
+      </c>
+      <c r="AZ20">
         <v>2</v>
       </c>
       <c r="BB20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BD20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="BE20">
+        <v>5</v>
+      </c>
+      <c r="BG20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43915</v>
       </c>
@@ -1216,32 +1242,32 @@
       <c r="AU21">
         <v>3</v>
       </c>
-      <c r="AV21">
-        <v>1</v>
-      </c>
       <c r="AW21">
-        <v>2</v>
-      </c>
-      <c r="AX21">
-        <v>1</v>
-      </c>
-      <c r="AY21">
+        <v>1</v>
+      </c>
+      <c r="AZ21">
         <v>2</v>
       </c>
       <c r="BA21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB21">
-        <v>5</v>
-      </c>
-      <c r="BC21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BD21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="BE21">
+        <v>5</v>
+      </c>
+      <c r="BF21">
+        <v>1</v>
+      </c>
+      <c r="BG21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43916</v>
       </c>
@@ -1374,26 +1400,26 @@
       <c r="AU22">
         <v>5</v>
       </c>
-      <c r="AV22">
-        <v>1</v>
-      </c>
       <c r="AW22">
-        <v>2</v>
-      </c>
-      <c r="AY22">
-        <v>2</v>
-      </c>
-      <c r="BA22">
+        <v>1</v>
+      </c>
+      <c r="AZ22">
         <v>2</v>
       </c>
       <c r="BB22">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BD22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="BE22">
+        <v>5</v>
+      </c>
+      <c r="BG22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43917</v>
       </c>
@@ -1502,26 +1528,26 @@
       <c r="AU23">
         <v>6</v>
       </c>
-      <c r="AV23">
-        <v>2</v>
-      </c>
       <c r="AW23">
-        <v>3</v>
-      </c>
-      <c r="AY23">
-        <v>2</v>
-      </c>
-      <c r="BA23">
+        <v>2</v>
+      </c>
+      <c r="AZ23">
         <v>3</v>
       </c>
       <c r="BB23">
+        <v>2</v>
+      </c>
+      <c r="BD23">
+        <v>3</v>
+      </c>
+      <c r="BE23">
         <v>6</v>
       </c>
-      <c r="BD23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BG23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43918</v>
       </c>
@@ -1660,26 +1686,26 @@
       <c r="AU24">
         <v>10</v>
       </c>
-      <c r="AV24">
-        <v>2</v>
-      </c>
       <c r="AW24">
-        <v>4</v>
-      </c>
-      <c r="AY24">
-        <v>2</v>
-      </c>
-      <c r="BA24">
+        <v>2</v>
+      </c>
+      <c r="AZ24">
         <v>4</v>
       </c>
       <c r="BB24">
+        <v>2</v>
+      </c>
+      <c r="BD24">
+        <v>4</v>
+      </c>
+      <c r="BE24">
         <v>7</v>
       </c>
-      <c r="BD24">
+      <c r="BG24">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43919</v>
       </c>
@@ -1788,26 +1814,26 @@
       <c r="AU25">
         <v>10</v>
       </c>
-      <c r="AV25">
-        <v>2</v>
-      </c>
       <c r="AW25">
-        <v>4</v>
-      </c>
-      <c r="AY25">
-        <v>3</v>
-      </c>
-      <c r="BA25">
+        <v>2</v>
+      </c>
+      <c r="AZ25">
         <v>4</v>
       </c>
       <c r="BB25">
+        <v>3</v>
+      </c>
+      <c r="BD25">
+        <v>4</v>
+      </c>
+      <c r="BE25">
         <v>7</v>
       </c>
-      <c r="BD25">
+      <c r="BG25">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43920</v>
       </c>
@@ -1946,26 +1972,26 @@
       <c r="AU26">
         <v>11</v>
       </c>
-      <c r="AV26">
-        <v>4</v>
-      </c>
       <c r="AW26">
         <v>4</v>
       </c>
-      <c r="AY26">
-        <v>4</v>
-      </c>
-      <c r="BA26">
+      <c r="AZ26">
         <v>4</v>
       </c>
       <c r="BB26">
+        <v>4</v>
+      </c>
+      <c r="BD26">
+        <v>4</v>
+      </c>
+      <c r="BE26">
         <v>10</v>
       </c>
-      <c r="BD26">
+      <c r="BG26">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43921</v>
       </c>
@@ -2101,29 +2127,29 @@
       <c r="AU27">
         <v>8</v>
       </c>
-      <c r="AV27">
-        <v>3</v>
-      </c>
       <c r="AW27">
-        <v>4</v>
-      </c>
-      <c r="AY27">
-        <v>5</v>
-      </c>
-      <c r="BA27">
+        <v>3</v>
+      </c>
+      <c r="AZ27">
         <v>4</v>
       </c>
       <c r="BB27">
+        <v>5</v>
+      </c>
+      <c r="BD27">
+        <v>4</v>
+      </c>
+      <c r="BE27">
         <v>11</v>
       </c>
-      <c r="BD27">
+      <c r="BG27">
         <v>17</v>
       </c>
-      <c r="BE27">
+      <c r="BI27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43922</v>
       </c>
@@ -2262,35 +2288,38 @@
       <c r="AU28">
         <v>9</v>
       </c>
-      <c r="AV28">
+      <c r="AW28">
         <v>6</v>
       </c>
-      <c r="AW28">
-        <v>4</v>
-      </c>
-      <c r="AY28">
+      <c r="AZ28">
+        <v>4</v>
+      </c>
+      <c r="BB28">
         <v>8</v>
       </c>
-      <c r="AZ28">
-        <v>1</v>
-      </c>
-      <c r="BA28">
-        <v>4</v>
-      </c>
-      <c r="BB28">
+      <c r="BC28">
+        <v>1</v>
+      </c>
+      <c r="BD28">
+        <v>4</v>
+      </c>
+      <c r="BE28">
         <v>12</v>
       </c>
-      <c r="BD28">
+      <c r="BG28">
         <v>18</v>
       </c>
-      <c r="BE28">
+      <c r="BI28">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43923</v>
       </c>
+      <c r="B29" s="2">
+        <v>1882</v>
+      </c>
       <c r="C29">
         <v>966</v>
       </c>
@@ -2426,29 +2455,208 @@
       <c r="AU29">
         <v>9</v>
       </c>
-      <c r="AV29">
-        <v>6</v>
-      </c>
       <c r="AW29">
         <v>6</v>
       </c>
-      <c r="AY29">
+      <c r="AZ29">
+        <v>6</v>
+      </c>
+      <c r="BB29">
         <v>8</v>
       </c>
-      <c r="AZ29">
-        <v>2</v>
-      </c>
-      <c r="BA29">
-        <v>4</v>
-      </c>
-      <c r="BB29">
+      <c r="BC29">
+        <v>2</v>
+      </c>
+      <c r="BD29">
+        <v>4</v>
+      </c>
+      <c r="BE29">
         <v>14</v>
       </c>
-      <c r="BD29">
+      <c r="BG29">
         <v>21</v>
       </c>
-      <c r="BE29">
+      <c r="BI29">
         <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>43924</v>
+      </c>
+      <c r="C30">
+        <v>1112</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>12</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>198</v>
+      </c>
+      <c r="I30">
+        <v>11</v>
+      </c>
+      <c r="J30">
+        <v>238</v>
+      </c>
+      <c r="K30">
+        <v>25</v>
+      </c>
+      <c r="L30">
+        <v>192</v>
+      </c>
+      <c r="M30">
+        <v>29</v>
+      </c>
+      <c r="N30">
+        <v>177</v>
+      </c>
+      <c r="O30">
+        <v>35</v>
+      </c>
+      <c r="P30">
+        <v>136</v>
+      </c>
+      <c r="Q30">
+        <v>41</v>
+      </c>
+      <c r="R30">
+        <v>88</v>
+      </c>
+      <c r="S30">
+        <v>34</v>
+      </c>
+      <c r="T30">
+        <v>55</v>
+      </c>
+      <c r="U30">
+        <v>33</v>
+      </c>
+      <c r="V30">
+        <v>6</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>519</v>
+      </c>
+      <c r="Y30">
+        <v>585</v>
+      </c>
+      <c r="Z30">
+        <v>8</v>
+      </c>
+      <c r="AA30">
+        <v>211</v>
+      </c>
+      <c r="AB30">
+        <v>85</v>
+      </c>
+      <c r="AC30">
+        <v>17</v>
+      </c>
+      <c r="AD30">
+        <v>37</v>
+      </c>
+      <c r="AE30">
+        <v>75</v>
+      </c>
+      <c r="AF30">
+        <v>4</v>
+      </c>
+      <c r="AG30">
+        <v>7</v>
+      </c>
+      <c r="AH30">
+        <v>60</v>
+      </c>
+      <c r="AI30">
+        <v>27</v>
+      </c>
+      <c r="AJ30">
+        <v>26</v>
+      </c>
+      <c r="AK30">
+        <v>2</v>
+      </c>
+      <c r="AL30">
+        <v>15</v>
+      </c>
+      <c r="AM30">
+        <v>10</v>
+      </c>
+      <c r="AN30">
+        <v>18</v>
+      </c>
+      <c r="AO30">
+        <v>27</v>
+      </c>
+      <c r="AP30">
+        <v>13</v>
+      </c>
+      <c r="AQ30">
+        <v>614</v>
+      </c>
+      <c r="AR30">
+        <v>13</v>
+      </c>
+      <c r="AS30">
+        <v>12</v>
+      </c>
+      <c r="AT30">
+        <v>5</v>
+      </c>
+      <c r="AU30">
+        <v>15</v>
+      </c>
+      <c r="AV30">
+        <v>1</v>
+      </c>
+      <c r="AW30">
+        <v>7</v>
+      </c>
+      <c r="AX30">
+        <v>1</v>
+      </c>
+      <c r="AY30">
+        <v>1</v>
+      </c>
+      <c r="AZ30">
+        <v>5</v>
+      </c>
+      <c r="BA30">
+        <v>1</v>
+      </c>
+      <c r="BB30">
+        <v>8</v>
+      </c>
+      <c r="BC30">
+        <v>2</v>
+      </c>
+      <c r="BD30">
+        <v>6</v>
+      </c>
+      <c r="BE30">
+        <v>13</v>
+      </c>
+      <c r="BG30">
+        <v>23</v>
+      </c>
+      <c r="BH30">
+        <v>1</v>
+      </c>
+      <c r="BI30">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data from Apr 5
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADA7FD2-1CEE-1946-A846-9831B68DFEB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D362BDA-A348-B54F-88A9-9070F229C0ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-19000" yWindow="-3600" windowWidth="19000" windowHeight="21600" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>date</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>valleycenter</t>
+  </si>
+  <si>
+    <t>sd_80plus_hosp</t>
   </si>
 </sst>
 </file>
@@ -566,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BI30"/>
+  <dimension ref="A1:BI32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Y30" sqref="Y30"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="BJ32" sqref="BJ32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,7 +648,7 @@
         <v>10</v>
       </c>
       <c r="U1" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="V1" t="s">
         <v>13</v>
@@ -2484,6 +2487,9 @@
       <c r="A30" s="1">
         <v>43924</v>
       </c>
+      <c r="B30" s="2">
+        <v>1025</v>
+      </c>
       <c r="C30">
         <v>1112</v>
       </c>
@@ -2657,6 +2663,337 @@
       </c>
       <c r="BI30">
         <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>43925</v>
+      </c>
+      <c r="B31" s="2">
+        <v>807</v>
+      </c>
+      <c r="C31">
+        <v>1209</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>14</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <v>209</v>
+      </c>
+      <c r="I31">
+        <v>13</v>
+      </c>
+      <c r="J31">
+        <v>251</v>
+      </c>
+      <c r="K31">
+        <v>26</v>
+      </c>
+      <c r="L31">
+        <v>212</v>
+      </c>
+      <c r="M31">
+        <v>30</v>
+      </c>
+      <c r="N31">
+        <v>202</v>
+      </c>
+      <c r="O31">
+        <v>41</v>
+      </c>
+      <c r="P31">
+        <v>152</v>
+      </c>
+      <c r="Q31">
+        <v>43</v>
+      </c>
+      <c r="R31">
+        <v>91</v>
+      </c>
+      <c r="S31">
+        <v>36</v>
+      </c>
+      <c r="T31">
+        <v>64</v>
+      </c>
+      <c r="U31">
+        <v>36</v>
+      </c>
+      <c r="V31">
+        <v>4</v>
+      </c>
+      <c r="W31">
+        <v>1</v>
+      </c>
+      <c r="X31">
+        <v>570</v>
+      </c>
+      <c r="Y31">
+        <v>630</v>
+      </c>
+      <c r="Z31">
+        <v>9</v>
+      </c>
+      <c r="AA31">
+        <v>228</v>
+      </c>
+      <c r="AB31">
+        <v>89</v>
+      </c>
+      <c r="AC31">
+        <v>18</v>
+      </c>
+      <c r="AD31">
+        <v>39</v>
+      </c>
+      <c r="AE31">
+        <v>86</v>
+      </c>
+      <c r="AF31">
+        <v>4</v>
+      </c>
+      <c r="AG31">
+        <v>7</v>
+      </c>
+      <c r="AH31">
+        <v>67</v>
+      </c>
+      <c r="AI31">
+        <v>27</v>
+      </c>
+      <c r="AJ31">
+        <v>27</v>
+      </c>
+      <c r="AK31">
+        <v>3</v>
+      </c>
+      <c r="AL31">
+        <v>18</v>
+      </c>
+      <c r="AM31">
+        <v>13</v>
+      </c>
+      <c r="AN31">
+        <v>18</v>
+      </c>
+      <c r="AO31">
+        <v>29</v>
+      </c>
+      <c r="AP31">
+        <v>13</v>
+      </c>
+      <c r="AQ31">
+        <v>649</v>
+      </c>
+      <c r="AR31">
+        <v>17</v>
+      </c>
+      <c r="AS31">
+        <v>15</v>
+      </c>
+      <c r="AT31">
+        <v>5</v>
+      </c>
+      <c r="AU31">
+        <v>17</v>
+      </c>
+      <c r="AV31">
+        <v>1</v>
+      </c>
+      <c r="AW31">
+        <v>8</v>
+      </c>
+      <c r="AX31">
+        <v>1</v>
+      </c>
+      <c r="AY31">
+        <v>1</v>
+      </c>
+      <c r="AZ31">
+        <v>6</v>
+      </c>
+      <c r="BA31">
+        <v>1</v>
+      </c>
+      <c r="BB31">
+        <v>9</v>
+      </c>
+      <c r="BC31">
+        <v>2</v>
+      </c>
+      <c r="BD31">
+        <v>7</v>
+      </c>
+      <c r="BE31">
+        <v>14</v>
+      </c>
+      <c r="BG31">
+        <v>27</v>
+      </c>
+      <c r="BH31">
+        <v>3</v>
+      </c>
+      <c r="BI31">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>43926</v>
+      </c>
+      <c r="C32">
+        <v>1326</v>
+      </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>15</v>
+      </c>
+      <c r="H32">
+        <v>226</v>
+      </c>
+      <c r="J32">
+        <v>286</v>
+      </c>
+      <c r="L32">
+        <v>237</v>
+      </c>
+      <c r="N32">
+        <v>222</v>
+      </c>
+      <c r="P32">
+        <v>162</v>
+      </c>
+      <c r="R32">
+        <v>99</v>
+      </c>
+      <c r="T32">
+        <v>66</v>
+      </c>
+      <c r="V32">
+        <v>3</v>
+      </c>
+      <c r="X32">
+        <v>609</v>
+      </c>
+      <c r="Y32">
+        <v>710</v>
+      </c>
+      <c r="Z32">
+        <v>7</v>
+      </c>
+      <c r="AA32">
+        <v>249</v>
+      </c>
+      <c r="AB32">
+        <v>94</v>
+      </c>
+      <c r="AC32">
+        <v>19</v>
+      </c>
+      <c r="AD32">
+        <v>41</v>
+      </c>
+      <c r="AE32">
+        <v>95</v>
+      </c>
+      <c r="AF32">
+        <v>4</v>
+      </c>
+      <c r="AG32">
+        <v>8</v>
+      </c>
+      <c r="AH32">
+        <v>72</v>
+      </c>
+      <c r="AI32">
+        <v>29</v>
+      </c>
+      <c r="AJ32">
+        <v>28</v>
+      </c>
+      <c r="AK32">
+        <v>6</v>
+      </c>
+      <c r="AL32">
+        <v>18</v>
+      </c>
+      <c r="AM32">
+        <v>12</v>
+      </c>
+      <c r="AN32">
+        <v>19</v>
+      </c>
+      <c r="AO32">
+        <v>30</v>
+      </c>
+      <c r="AP32">
+        <v>13</v>
+      </c>
+      <c r="AQ32">
+        <v>686</v>
+      </c>
+      <c r="AR32">
+        <v>17</v>
+      </c>
+      <c r="AS32">
+        <v>16</v>
+      </c>
+      <c r="AT32">
+        <v>5</v>
+      </c>
+      <c r="AU32">
+        <v>18</v>
+      </c>
+      <c r="AV32">
+        <v>1</v>
+      </c>
+      <c r="AW32">
+        <v>8</v>
+      </c>
+      <c r="AX32">
+        <v>1</v>
+      </c>
+      <c r="AY32">
+        <v>1</v>
+      </c>
+      <c r="AZ32">
+        <v>6</v>
+      </c>
+      <c r="BA32">
+        <v>1</v>
+      </c>
+      <c r="BB32">
+        <v>10</v>
+      </c>
+      <c r="BC32">
+        <v>2</v>
+      </c>
+      <c r="BD32">
+        <v>7</v>
+      </c>
+      <c r="BE32">
+        <v>14</v>
+      </c>
+      <c r="BG32">
+        <v>28</v>
+      </c>
+      <c r="BH32">
+        <v>3</v>
+      </c>
+      <c r="BI32">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data from Apr 6
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D362BDA-A348-B54F-88A9-9070F229C0ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72894F1-3567-E84B-B781-842094D03049}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19000" yWindow="-3600" windowWidth="19000" windowHeight="21600" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="19160" windowHeight="21600" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BI32"/>
+  <dimension ref="A1:BI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BJ32" sqref="BJ32"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BK34" sqref="BK34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2851,6 +2851,9 @@
       <c r="A32" s="1">
         <v>43926</v>
       </c>
+      <c r="B32" s="2">
+        <v>827</v>
+      </c>
       <c r="C32">
         <v>1326</v>
       </c>
@@ -2994,6 +2997,155 @@
       </c>
       <c r="BI32">
         <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>43927</v>
+      </c>
+      <c r="C33">
+        <v>1404</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>15</v>
+      </c>
+      <c r="H33">
+        <v>235</v>
+      </c>
+      <c r="J33">
+        <v>300</v>
+      </c>
+      <c r="L33">
+        <v>254</v>
+      </c>
+      <c r="N33">
+        <v>235</v>
+      </c>
+      <c r="P33">
+        <v>172</v>
+      </c>
+      <c r="R33">
+        <v>109</v>
+      </c>
+      <c r="T33">
+        <v>71</v>
+      </c>
+      <c r="V33">
+        <v>3</v>
+      </c>
+      <c r="X33">
+        <v>657</v>
+      </c>
+      <c r="Y33">
+        <v>739</v>
+      </c>
+      <c r="Z33">
+        <v>8</v>
+      </c>
+      <c r="AA33">
+        <v>269</v>
+      </c>
+      <c r="AB33">
+        <v>102</v>
+      </c>
+      <c r="AC33">
+        <v>19</v>
+      </c>
+      <c r="AD33">
+        <v>42</v>
+      </c>
+      <c r="AE33">
+        <v>104</v>
+      </c>
+      <c r="AF33">
+        <v>4</v>
+      </c>
+      <c r="AG33">
+        <v>8</v>
+      </c>
+      <c r="AH33">
+        <v>74</v>
+      </c>
+      <c r="AI33">
+        <v>30</v>
+      </c>
+      <c r="AJ33">
+        <v>28</v>
+      </c>
+      <c r="AK33">
+        <v>7</v>
+      </c>
+      <c r="AL33">
+        <v>23</v>
+      </c>
+      <c r="AM33">
+        <v>13</v>
+      </c>
+      <c r="AN33">
+        <v>25</v>
+      </c>
+      <c r="AO33">
+        <v>31</v>
+      </c>
+      <c r="AP33">
+        <v>14</v>
+      </c>
+      <c r="AQ33">
+        <v>713</v>
+      </c>
+      <c r="AR33">
+        <v>19</v>
+      </c>
+      <c r="AS33">
+        <v>16</v>
+      </c>
+      <c r="AT33">
+        <v>5</v>
+      </c>
+      <c r="AU33">
+        <v>21</v>
+      </c>
+      <c r="AV33">
+        <v>1</v>
+      </c>
+      <c r="AW33">
+        <v>8</v>
+      </c>
+      <c r="AX33">
+        <v>1</v>
+      </c>
+      <c r="AY33">
+        <v>1</v>
+      </c>
+      <c r="AZ33">
+        <v>6</v>
+      </c>
+      <c r="BA33">
+        <v>2</v>
+      </c>
+      <c r="BB33">
+        <v>12</v>
+      </c>
+      <c r="BC33">
+        <v>2</v>
+      </c>
+      <c r="BD33">
+        <v>8</v>
+      </c>
+      <c r="BE33">
+        <v>14</v>
+      </c>
+      <c r="BG33">
+        <v>34</v>
+      </c>
+      <c r="BH33">
+        <v>3</v>
+      </c>
+      <c r="BI33">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update from Apr 7
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72894F1-3567-E84B-B781-842094D03049}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65904DD5-4E73-5D44-8586-C8F64E7CE924}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="19160" windowHeight="21600" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BI33"/>
+  <dimension ref="A1:BI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BK34" sqref="BK34"/>
+    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="BJ34" sqref="BJ34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3003,6 +3003,9 @@
       <c r="A33" s="1">
         <v>43927</v>
       </c>
+      <c r="B33" s="2">
+        <v>1846</v>
+      </c>
       <c r="C33">
         <v>1404</v>
       </c>
@@ -3146,6 +3149,155 @@
       </c>
       <c r="BI33">
         <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>43928</v>
+      </c>
+      <c r="C34">
+        <v>1454</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <v>16</v>
+      </c>
+      <c r="H34">
+        <v>240</v>
+      </c>
+      <c r="J34">
+        <v>288</v>
+      </c>
+      <c r="L34">
+        <v>259</v>
+      </c>
+      <c r="N34">
+        <v>255</v>
+      </c>
+      <c r="P34">
+        <v>190</v>
+      </c>
+      <c r="R34">
+        <v>115</v>
+      </c>
+      <c r="T34">
+        <v>79</v>
+      </c>
+      <c r="V34">
+        <v>2</v>
+      </c>
+      <c r="X34">
+        <v>701</v>
+      </c>
+      <c r="Y34">
+        <v>747</v>
+      </c>
+      <c r="Z34">
+        <v>6</v>
+      </c>
+      <c r="AA34">
+        <v>289</v>
+      </c>
+      <c r="AB34">
+        <v>109</v>
+      </c>
+      <c r="AC34">
+        <v>31</v>
+      </c>
+      <c r="AD34">
+        <v>42</v>
+      </c>
+      <c r="AE34">
+        <v>120</v>
+      </c>
+      <c r="AF34">
+        <v>4</v>
+      </c>
+      <c r="AG34">
+        <v>8</v>
+      </c>
+      <c r="AH34">
+        <v>85</v>
+      </c>
+      <c r="AI34">
+        <v>31</v>
+      </c>
+      <c r="AJ34">
+        <v>32</v>
+      </c>
+      <c r="AK34">
+        <v>7</v>
+      </c>
+      <c r="AL34">
+        <v>25</v>
+      </c>
+      <c r="AM34">
+        <v>14</v>
+      </c>
+      <c r="AN34">
+        <v>25</v>
+      </c>
+      <c r="AO34">
+        <v>31</v>
+      </c>
+      <c r="AP34">
+        <v>15</v>
+      </c>
+      <c r="AQ34">
+        <v>750</v>
+      </c>
+      <c r="AR34">
+        <v>20</v>
+      </c>
+      <c r="AS34">
+        <v>14</v>
+      </c>
+      <c r="AT34">
+        <v>5</v>
+      </c>
+      <c r="AU34">
+        <v>22</v>
+      </c>
+      <c r="AV34">
+        <v>1</v>
+      </c>
+      <c r="AW34">
+        <v>11</v>
+      </c>
+      <c r="AX34">
+        <v>1</v>
+      </c>
+      <c r="AY34">
+        <v>1</v>
+      </c>
+      <c r="AZ34">
+        <v>6</v>
+      </c>
+      <c r="BA34">
+        <v>3</v>
+      </c>
+      <c r="BB34">
+        <v>14</v>
+      </c>
+      <c r="BC34">
+        <v>2</v>
+      </c>
+      <c r="BD34">
+        <v>9</v>
+      </c>
+      <c r="BE34">
+        <v>14</v>
+      </c>
+      <c r="BG34">
+        <v>34</v>
+      </c>
+      <c r="BH34">
+        <v>3</v>
+      </c>
+      <c r="BI34">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with data from Apr 9
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10405"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65904DD5-4E73-5D44-8586-C8F64E7CE924}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45366279-1E44-3F42-BFCD-27C588FAD191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-18720" yWindow="-3600" windowWidth="18720" windowHeight="21600" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BI34"/>
+  <dimension ref="A1:BI35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
-      <selection activeCell="BJ34" sqref="BJ34"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="BJ35" sqref="BJ35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3155,6 +3155,9 @@
       <c r="A34" s="1">
         <v>43928</v>
       </c>
+      <c r="B34" s="2">
+        <v>842</v>
+      </c>
       <c r="C34">
         <v>1454</v>
       </c>
@@ -3298,6 +3301,155 @@
       </c>
       <c r="BI34">
         <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>43929</v>
+      </c>
+      <c r="C35">
+        <v>1530</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <v>16</v>
+      </c>
+      <c r="H35">
+        <v>244</v>
+      </c>
+      <c r="J35">
+        <v>301</v>
+      </c>
+      <c r="L35">
+        <v>268</v>
+      </c>
+      <c r="N35">
+        <v>278</v>
+      </c>
+      <c r="P35">
+        <v>201</v>
+      </c>
+      <c r="R35">
+        <v>123</v>
+      </c>
+      <c r="T35">
+        <v>86</v>
+      </c>
+      <c r="V35">
+        <v>3</v>
+      </c>
+      <c r="X35">
+        <v>737</v>
+      </c>
+      <c r="Y35">
+        <v>785</v>
+      </c>
+      <c r="Z35">
+        <v>8</v>
+      </c>
+      <c r="AA35">
+        <v>316</v>
+      </c>
+      <c r="AB35">
+        <v>122</v>
+      </c>
+      <c r="AC35">
+        <v>36</v>
+      </c>
+      <c r="AD35">
+        <v>43</v>
+      </c>
+      <c r="AE35">
+        <v>133</v>
+      </c>
+      <c r="AF35">
+        <v>4</v>
+      </c>
+      <c r="AG35">
+        <v>8</v>
+      </c>
+      <c r="AH35">
+        <v>88</v>
+      </c>
+      <c r="AI35">
+        <v>32</v>
+      </c>
+      <c r="AJ35">
+        <v>35</v>
+      </c>
+      <c r="AK35">
+        <v>9</v>
+      </c>
+      <c r="AL35">
+        <v>29</v>
+      </c>
+      <c r="AM35">
+        <v>14</v>
+      </c>
+      <c r="AN35">
+        <v>28</v>
+      </c>
+      <c r="AO35">
+        <v>34</v>
+      </c>
+      <c r="AP35">
+        <v>16</v>
+      </c>
+      <c r="AQ35">
+        <v>783</v>
+      </c>
+      <c r="AR35">
+        <v>20</v>
+      </c>
+      <c r="AS35">
+        <v>16</v>
+      </c>
+      <c r="AT35">
+        <v>5</v>
+      </c>
+      <c r="AU35">
+        <v>24</v>
+      </c>
+      <c r="AV35">
+        <v>1</v>
+      </c>
+      <c r="AW35">
+        <v>13</v>
+      </c>
+      <c r="AX35">
+        <v>1</v>
+      </c>
+      <c r="AY35">
+        <v>1</v>
+      </c>
+      <c r="AZ35">
+        <v>6</v>
+      </c>
+      <c r="BA35">
+        <v>3</v>
+      </c>
+      <c r="BB35">
+        <v>14</v>
+      </c>
+      <c r="BC35">
+        <v>2</v>
+      </c>
+      <c r="BD35">
+        <v>10</v>
+      </c>
+      <c r="BE35">
+        <v>14</v>
+      </c>
+      <c r="BG35">
+        <v>37</v>
+      </c>
+      <c r="BH35">
+        <v>3</v>
+      </c>
+      <c r="BI35">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with data from Apr 10
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45366279-1E44-3F42-BFCD-27C588FAD191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C75F68C-9DEF-3149-84CC-C74782E8A2DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18720" yWindow="-3600" windowWidth="18720" windowHeight="21600" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BI35"/>
+  <dimension ref="A1:BI36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BJ35" sqref="BJ35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3307,6 +3307,9 @@
       <c r="A35" s="1">
         <v>43929</v>
       </c>
+      <c r="B35" s="2">
+        <v>920</v>
+      </c>
       <c r="C35">
         <v>1530</v>
       </c>
@@ -3450,6 +3453,155 @@
       </c>
       <c r="BI35">
         <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>43930</v>
+      </c>
+      <c r="C36">
+        <v>1628</v>
+      </c>
+      <c r="D36">
+        <v>10</v>
+      </c>
+      <c r="F36">
+        <v>20</v>
+      </c>
+      <c r="H36">
+        <v>255</v>
+      </c>
+      <c r="J36">
+        <v>320</v>
+      </c>
+      <c r="L36">
+        <v>283</v>
+      </c>
+      <c r="N36">
+        <v>293</v>
+      </c>
+      <c r="P36">
+        <v>224</v>
+      </c>
+      <c r="R36">
+        <v>131</v>
+      </c>
+      <c r="T36">
+        <v>90</v>
+      </c>
+      <c r="V36">
+        <v>2</v>
+      </c>
+      <c r="X36">
+        <v>790</v>
+      </c>
+      <c r="Y36">
+        <v>832</v>
+      </c>
+      <c r="Z36">
+        <v>6</v>
+      </c>
+      <c r="AA36">
+        <v>348</v>
+      </c>
+      <c r="AB36">
+        <v>132</v>
+      </c>
+      <c r="AC36">
+        <v>40</v>
+      </c>
+      <c r="AD36">
+        <v>43</v>
+      </c>
+      <c r="AE36">
+        <v>154</v>
+      </c>
+      <c r="AF36">
+        <v>5</v>
+      </c>
+      <c r="AG36">
+        <v>8</v>
+      </c>
+      <c r="AH36">
+        <v>93</v>
+      </c>
+      <c r="AI36">
+        <v>32</v>
+      </c>
+      <c r="AJ36">
+        <v>39</v>
+      </c>
+      <c r="AK36">
+        <v>10</v>
+      </c>
+      <c r="AL36">
+        <v>30</v>
+      </c>
+      <c r="AM36">
+        <v>14</v>
+      </c>
+      <c r="AN36">
+        <v>32</v>
+      </c>
+      <c r="AO36">
+        <v>34</v>
+      </c>
+      <c r="AP36">
+        <v>16</v>
+      </c>
+      <c r="AQ36">
+        <v>821</v>
+      </c>
+      <c r="AR36">
+        <v>21</v>
+      </c>
+      <c r="AS36">
+        <v>17</v>
+      </c>
+      <c r="AT36">
+        <v>5</v>
+      </c>
+      <c r="AU36">
+        <v>26</v>
+      </c>
+      <c r="AV36">
+        <v>1</v>
+      </c>
+      <c r="AW36">
+        <v>13</v>
+      </c>
+      <c r="AX36">
+        <v>1</v>
+      </c>
+      <c r="AY36">
+        <v>1</v>
+      </c>
+      <c r="AZ36">
+        <v>7</v>
+      </c>
+      <c r="BA36">
+        <v>4</v>
+      </c>
+      <c r="BB36">
+        <v>13</v>
+      </c>
+      <c r="BC36">
+        <v>2</v>
+      </c>
+      <c r="BD36">
+        <v>10</v>
+      </c>
+      <c r="BE36">
+        <v>14</v>
+      </c>
+      <c r="BG36">
+        <v>39</v>
+      </c>
+      <c r="BH36">
+        <v>3</v>
+      </c>
+      <c r="BI36">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data from Apr 12 added
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CF8EDC-C8E9-2C46-9601-0E7DE43D5B0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93AB2B9-5E6C-3147-A85A-DF3E8BFA2FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BI37"/>
+  <dimension ref="A1:BI38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BI37" sqref="BI37"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3611,6 +3611,9 @@
       <c r="A37" s="1">
         <v>43931</v>
       </c>
+      <c r="B37" s="2">
+        <v>1077</v>
+      </c>
       <c r="C37">
         <v>1693</v>
       </c>
@@ -3754,6 +3757,62 @@
       </c>
       <c r="BI37">
         <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>43932</v>
+      </c>
+      <c r="C38">
+        <v>1761</v>
+      </c>
+      <c r="D38">
+        <v>10</v>
+      </c>
+      <c r="F38">
+        <v>22</v>
+      </c>
+      <c r="H38">
+        <v>270</v>
+      </c>
+      <c r="J38">
+        <v>343</v>
+      </c>
+      <c r="L38">
+        <v>304</v>
+      </c>
+      <c r="N38">
+        <v>318</v>
+      </c>
+      <c r="P38">
+        <v>245</v>
+      </c>
+      <c r="R38">
+        <v>143</v>
+      </c>
+      <c r="T38">
+        <v>104</v>
+      </c>
+      <c r="V38">
+        <v>2</v>
+      </c>
+      <c r="X38">
+        <v>853</v>
+      </c>
+      <c r="Y38">
+        <v>902</v>
+      </c>
+      <c r="Z38">
+        <v>6</v>
+      </c>
+      <c r="AA38">
+        <v>396</v>
+      </c>
+      <c r="AB38">
+        <v>144</v>
+      </c>
+      <c r="AC38">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data from April 12
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93AB2B9-5E6C-3147-A85A-DF3E8BFA2FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2302EB99-27D3-5548-A154-FF82596B54B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BI38"/>
+  <dimension ref="A1:BI39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3763,6 +3763,9 @@
       <c r="A38" s="1">
         <v>43932</v>
       </c>
+      <c r="B38" s="2">
+        <v>804</v>
+      </c>
       <c r="C38">
         <v>1761</v>
       </c>
@@ -3812,6 +3815,62 @@
         <v>144</v>
       </c>
       <c r="AC38">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>43933</v>
+      </c>
+      <c r="C39">
+        <v>1804</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+      <c r="F39">
+        <v>22</v>
+      </c>
+      <c r="H39">
+        <v>273</v>
+      </c>
+      <c r="J39">
+        <v>352</v>
+      </c>
+      <c r="L39">
+        <v>312</v>
+      </c>
+      <c r="N39">
+        <v>328</v>
+      </c>
+      <c r="P39">
+        <v>250</v>
+      </c>
+      <c r="R39">
+        <v>145</v>
+      </c>
+      <c r="T39">
+        <v>109</v>
+      </c>
+      <c r="V39">
+        <v>3</v>
+      </c>
+      <c r="X39">
+        <v>877</v>
+      </c>
+      <c r="Y39">
+        <v>922</v>
+      </c>
+      <c r="Z39">
+        <v>5</v>
+      </c>
+      <c r="AA39">
+        <v>415</v>
+      </c>
+      <c r="AB39">
+        <v>152</v>
+      </c>
+      <c r="AC39">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data from Apr 14
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2302EB99-27D3-5548-A154-FF82596B54B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD21056-64AE-C542-9F17-91644616058E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-19000" yWindow="-3600" windowWidth="19000" windowHeight="21600" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BI39"/>
+  <dimension ref="A1:BI41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3822,6 +3822,9 @@
       <c r="A39" s="1">
         <v>43933</v>
       </c>
+      <c r="B39" s="2">
+        <v>898</v>
+      </c>
       <c r="C39">
         <v>1804</v>
       </c>
@@ -3872,6 +3875,121 @@
       </c>
       <c r="AC39">
         <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>43934</v>
+      </c>
+      <c r="B40" s="2">
+        <v>919</v>
+      </c>
+      <c r="C40">
+        <v>1847</v>
+      </c>
+      <c r="D40">
+        <v>11</v>
+      </c>
+      <c r="F40">
+        <v>23</v>
+      </c>
+      <c r="H40">
+        <v>279</v>
+      </c>
+      <c r="J40">
+        <v>359</v>
+      </c>
+      <c r="L40">
+        <v>320</v>
+      </c>
+      <c r="N40">
+        <v>338</v>
+      </c>
+      <c r="P40">
+        <v>255</v>
+      </c>
+      <c r="R40">
+        <v>146</v>
+      </c>
+      <c r="T40">
+        <v>113</v>
+      </c>
+      <c r="V40">
+        <v>3</v>
+      </c>
+      <c r="X40">
+        <v>905</v>
+      </c>
+      <c r="Y40">
+        <v>937</v>
+      </c>
+      <c r="Z40">
+        <v>5</v>
+      </c>
+      <c r="AA40">
+        <v>420</v>
+      </c>
+      <c r="AB40">
+        <v>156</v>
+      </c>
+      <c r="AC40">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>43935</v>
+      </c>
+      <c r="C41">
+        <v>1930</v>
+      </c>
+      <c r="D41">
+        <v>12</v>
+      </c>
+      <c r="F41">
+        <v>24</v>
+      </c>
+      <c r="H41">
+        <v>292</v>
+      </c>
+      <c r="J41">
+        <v>367</v>
+      </c>
+      <c r="L41">
+        <v>339</v>
+      </c>
+      <c r="N41">
+        <v>352</v>
+      </c>
+      <c r="P41">
+        <v>265</v>
+      </c>
+      <c r="R41">
+        <v>155</v>
+      </c>
+      <c r="T41">
+        <v>121</v>
+      </c>
+      <c r="V41">
+        <v>3</v>
+      </c>
+      <c r="X41">
+        <v>954</v>
+      </c>
+      <c r="Y41">
+        <v>971</v>
+      </c>
+      <c r="Z41">
+        <v>5</v>
+      </c>
+      <c r="AA41">
+        <v>450</v>
+      </c>
+      <c r="AB41">
+        <v>164</v>
+      </c>
+      <c r="AC41">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data from Apr 15
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD21056-64AE-C542-9F17-91644616058E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0444D0-8E94-5043-88C7-E289F1DAC946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19000" yWindow="-3600" windowWidth="19000" windowHeight="21600" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="-37820" yWindow="-3140" windowWidth="19000" windowHeight="21140" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BI41"/>
+  <dimension ref="A1:BI42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3940,6 +3940,9 @@
       <c r="A41" s="1">
         <v>43935</v>
       </c>
+      <c r="B41" s="2">
+        <v>836</v>
+      </c>
       <c r="C41">
         <v>1930</v>
       </c>
@@ -3990,6 +3993,53 @@
       </c>
       <c r="AC41">
         <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>43936</v>
+      </c>
+      <c r="C42">
+        <v>2012</v>
+      </c>
+      <c r="D42">
+        <v>12</v>
+      </c>
+      <c r="F42">
+        <v>32</v>
+      </c>
+      <c r="H42">
+        <v>308</v>
+      </c>
+      <c r="J42">
+        <v>381</v>
+      </c>
+      <c r="L42">
+        <v>350</v>
+      </c>
+      <c r="N42">
+        <v>367</v>
+      </c>
+      <c r="P42">
+        <v>275</v>
+      </c>
+      <c r="R42">
+        <v>160</v>
+      </c>
+      <c r="T42">
+        <v>124</v>
+      </c>
+      <c r="V42">
+        <v>3</v>
+      </c>
+      <c r="X42">
+        <v>989</v>
+      </c>
+      <c r="Y42">
+        <v>1017</v>
+      </c>
+      <c r="Z42">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data from Apr 17
</commit_message>
<xml_diff>
--- a/sd_covid_dataset.xlsx
+++ b/sd_covid_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menis/local.work/learning/covid/sd_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0444D0-8E94-5043-88C7-E289F1DAC946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A153F8-5FEF-EE4A-8E00-4F1F4E52D240}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37820" yWindow="-3140" windowWidth="19000" windowHeight="21140" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
+    <workbookView xWindow="1560" yWindow="460" windowWidth="19000" windowHeight="17540" xr2:uid="{90E28514-B523-EF42-8F4B-F0DCEDFCF387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4869025C-BFFA-184C-850E-A77257F132C8}">
-  <dimension ref="A1:BI42"/>
+  <dimension ref="A1:BI44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3999,6 +3999,9 @@
       <c r="A42" s="1">
         <v>43936</v>
       </c>
+      <c r="B42" s="2">
+        <v>1248</v>
+      </c>
       <c r="C42">
         <v>2012</v>
       </c>
@@ -4040,6 +4043,130 @@
       </c>
       <c r="Z42">
         <v>6</v>
+      </c>
+      <c r="AA42">
+        <v>480</v>
+      </c>
+      <c r="AB42">
+        <v>170</v>
+      </c>
+      <c r="AC42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1114</v>
+      </c>
+      <c r="C43">
+        <v>2087</v>
+      </c>
+      <c r="D43">
+        <v>12</v>
+      </c>
+      <c r="F43">
+        <v>34</v>
+      </c>
+      <c r="H43">
+        <v>316</v>
+      </c>
+      <c r="J43">
+        <v>399</v>
+      </c>
+      <c r="L43">
+        <v>362</v>
+      </c>
+      <c r="N43">
+        <v>383</v>
+      </c>
+      <c r="P43">
+        <v>286</v>
+      </c>
+      <c r="R43">
+        <v>163</v>
+      </c>
+      <c r="T43">
+        <v>129</v>
+      </c>
+      <c r="V43">
+        <v>3</v>
+      </c>
+      <c r="X43">
+        <v>1034</v>
+      </c>
+      <c r="Y43">
+        <v>1047</v>
+      </c>
+      <c r="Z43">
+        <v>6</v>
+      </c>
+      <c r="AA43">
+        <v>507</v>
+      </c>
+      <c r="AB43">
+        <v>181</v>
+      </c>
+      <c r="AC43">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>43938</v>
+      </c>
+      <c r="C44">
+        <v>2158</v>
+      </c>
+      <c r="D44">
+        <v>13</v>
+      </c>
+      <c r="F44">
+        <v>35</v>
+      </c>
+      <c r="H44">
+        <v>327</v>
+      </c>
+      <c r="J44">
+        <v>408</v>
+      </c>
+      <c r="L44">
+        <v>373</v>
+      </c>
+      <c r="N44">
+        <v>404</v>
+      </c>
+      <c r="P44">
+        <v>297</v>
+      </c>
+      <c r="R44">
+        <v>166</v>
+      </c>
+      <c r="T44">
+        <v>131</v>
+      </c>
+      <c r="V44">
+        <v>4</v>
+      </c>
+      <c r="X44">
+        <v>1073</v>
+      </c>
+      <c r="Y44">
+        <v>1081</v>
+      </c>
+      <c r="Z44">
+        <v>4</v>
+      </c>
+      <c r="AA44">
+        <v>524</v>
+      </c>
+      <c r="AB44">
+        <v>181</v>
+      </c>
+      <c r="AC44">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>